<commit_message>
Backup: Wed Jan  1 16:49:30 IST 2025
</commit_message>
<xml_diff>
--- a/linear_regression_with_significance.xlsx
+++ b/linear_regression_with_significance.xlsx
@@ -28,276 +28,279 @@
     <t>P-value</t>
   </si>
   <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
     <t>Lateral Occipital Cortex, superior division Volume Change</t>
   </si>
   <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Change</t>
+    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age at baseline </t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
   </si>
   <si>
     <t>Frontal Pole Volume Change</t>
   </si>
   <si>
-    <t>Occipital Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Change</t>
+    <t>Temporal Fusiform Cortex, posterior division Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Change</t>
+  </si>
+  <si>
+    <t>Frontal Pole Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Change</t>
   </si>
   <si>
     <t>Frontal Medial Cortex Volume Change</t>
   </si>
   <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age at baseline </t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Change</t>
-  </si>
-  <si>
     <t>Paracingulate Gyrus Change</t>
   </si>
   <si>
@@ -305,9 +308,6 @@
   </si>
   <si>
     <t>Parahippocampal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
   </si>
   <si>
     <t>Central Opercular Cortex Change</t>
@@ -702,13 +702,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>63.07813883944394</v>
+        <v>39.6969084606372</v>
       </c>
       <c r="C2">
-        <v>0.08138632758091358</v>
+        <v>0.4218896826120796</v>
       </c>
       <c r="D2">
-        <v>0.1411677803662266</v>
+        <v>0.01327284346805847</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -716,13 +716,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>63.45574012761816</v>
+        <v>61.86812217071104</v>
       </c>
       <c r="C3">
-        <v>0.07588727969488129</v>
+        <v>0.09900792955275184</v>
       </c>
       <c r="D3">
-        <v>0.1963225346088467</v>
+        <v>0.1676739325884186</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -730,13 +730,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>64.08182761927326</v>
+        <v>66.12200276610442</v>
       </c>
       <c r="C4">
-        <v>0.06676950069019538</v>
+        <v>0.03705821214411043</v>
       </c>
       <c r="D4">
-        <v>0.1734095385432013</v>
+        <v>0.09346911303928794</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -744,13 +744,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>64.41252930566229</v>
+        <v>66.98652591476593</v>
       </c>
       <c r="C5">
-        <v>0.06195345671365604</v>
+        <v>0.02446806920243783</v>
       </c>
       <c r="D5">
-        <v>0.1007251654754354</v>
+        <v>0.4556668748933871</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -758,13 +758,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>65.85179132678552</v>
+        <v>67.64606448730302</v>
       </c>
       <c r="C6">
-        <v>0.040993330192444</v>
+        <v>0.01486313853442212</v>
       </c>
       <c r="D6">
-        <v>0.3846752521144173</v>
+        <v>0.4604050421945982</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -772,13 +772,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>66.50655169422492</v>
+        <v>67.8513832008049</v>
       </c>
       <c r="C7">
-        <v>0.03145798503555941</v>
+        <v>0.01187306018245293</v>
       </c>
       <c r="D7">
-        <v>0.2900839752743882</v>
+        <v>0.4956594214689176</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -786,13 +786,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>66.98652591476593</v>
+        <v>68.07909947890576</v>
       </c>
       <c r="C8">
-        <v>0.02446806920243783</v>
+        <v>0.008556803705255911</v>
       </c>
       <c r="D8">
-        <v>0.4556668748933871</v>
+        <v>0.06318905803758798</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -800,13 +800,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>68.66723356009069</v>
+        <v>68.48992841584712</v>
       </c>
       <c r="C9">
-        <v>-8.255729476269735E-06</v>
+        <v>0.002573858021644004</v>
       </c>
       <c r="D9">
-        <v>0.1246300918071437</v>
+        <v>0.3186013917789818</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -814,13 +814,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>68.85444444444445</v>
+        <v>68.66766388657908</v>
       </c>
       <c r="C10">
-        <v>-0.002734627831715297</v>
+        <v>-1.452262008383443E-05</v>
       </c>
       <c r="D10">
-        <v>0.7220787472790002</v>
+        <v>0.2675875235013904</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -828,13 +828,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>68.98895941840277</v>
+        <v>68.85444444444445</v>
       </c>
       <c r="C11">
-        <v>-0.004693583763147213</v>
+        <v>-0.002734627831715297</v>
       </c>
       <c r="D11">
-        <v>0.4323342465057807</v>
+        <v>0.7220787472790002</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -842,13 +842,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>69.00694444444444</v>
+        <v>68.90581617919213</v>
       </c>
       <c r="C12">
-        <v>-0.004955501618123082</v>
+        <v>-0.003482759891147547</v>
       </c>
       <c r="D12">
-        <v>0.4703983292785431</v>
+        <v>0.7303388057829046</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -856,13 +856,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>69.02623836670939</v>
+        <v>69.01826504146955</v>
       </c>
       <c r="C13">
-        <v>-0.005236481068583432</v>
+        <v>-0.00512036468159538</v>
       </c>
       <c r="D13">
-        <v>0.3843926379216691</v>
+        <v>0.4031055848774701</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -870,13 +870,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>69.11276880006525</v>
+        <v>69.06355495859624</v>
       </c>
       <c r="C14">
-        <v>-0.006496633010659059</v>
+        <v>-0.005779926581498618</v>
       </c>
       <c r="D14">
-        <v>0.8029550276097792</v>
+        <v>0.2040618196925583</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -884,13 +884,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>69.13824000939569</v>
+        <v>69.10255892610388</v>
       </c>
       <c r="C15">
-        <v>-0.006867572952364398</v>
+        <v>-0.006347945525784882</v>
       </c>
       <c r="D15">
-        <v>0.5565832971759981</v>
+        <v>0.3340370223553067</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -898,13 +898,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>69.17526973011793</v>
+        <v>69.13824000939569</v>
       </c>
       <c r="C16">
-        <v>-0.007406840729872854</v>
+        <v>-0.006867572952364398</v>
       </c>
       <c r="D16">
-        <v>0.7674567629563238</v>
+        <v>0.5565832971759981</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -912,13 +912,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>69.19919947879916</v>
+        <v>69.14638220513085</v>
       </c>
       <c r="C17">
-        <v>-0.007755332215521715</v>
+        <v>-0.006986148618410404</v>
       </c>
       <c r="D17">
-        <v>0.8319367723094866</v>
+        <v>0.4569685920449683</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -926,13 +926,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>69.23475372000667</v>
+        <v>69.2027704034229</v>
       </c>
       <c r="C18">
-        <v>-0.008273112427281459</v>
+        <v>-0.007807335972178198</v>
       </c>
       <c r="D18">
-        <v>0.9696551077742305</v>
+        <v>0.4487351500627458</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -940,10 +940,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>69.24058769513314</v>
+        <v>69.22075130267341</v>
       </c>
       <c r="C19">
-        <v>-0.008358073230094298</v>
+        <v>-0.008069193728253543</v>
+      </c>
+      <c r="D19">
+        <v>0.9477832899558639</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -951,10 +954,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>69.24058769513314</v>
+        <v>69.24781957267116</v>
       </c>
       <c r="C20">
-        <v>-0.008358073230094298</v>
+        <v>-0.008463391835016765</v>
+      </c>
+      <c r="D20">
+        <v>0.766764388878391</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -962,10 +968,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>69.24058769513314</v>
+        <v>69.26387073719739</v>
       </c>
       <c r="C21">
-        <v>-0.008358073230094298</v>
+        <v>-0.008697146658214416</v>
+      </c>
+      <c r="D21">
+        <v>0.5094561817189306</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -973,10 +982,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>69.24058769513314</v>
+        <v>69.31002826128042</v>
       </c>
       <c r="C22">
-        <v>-0.008358073230094298</v>
+        <v>-0.009369343610879932</v>
+      </c>
+      <c r="D22">
+        <v>0.9494539888673468</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -984,13 +996,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>69.2513208629894</v>
+        <v>69.56447608405639</v>
       </c>
       <c r="C23">
-        <v>-0.008514381499845625</v>
+        <v>-0.01307489442800569</v>
       </c>
       <c r="D23">
-        <v>0.7776079721842161</v>
+        <v>0.08599038957451426</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -998,13 +1010,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>69.25421609734047</v>
+        <v>69.56874263372083</v>
       </c>
       <c r="C24">
-        <v>-0.008556545106900293</v>
+        <v>-0.01313702864641986</v>
       </c>
       <c r="D24">
-        <v>0.3602285534130157</v>
+        <v>0.9619947627823591</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1012,13 +1024,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>69.257746560296</v>
+        <v>69.57062689014457</v>
       </c>
       <c r="C25">
-        <v>-0.008607959615961169</v>
+        <v>-0.0131644692739501</v>
       </c>
       <c r="D25">
-        <v>0.9982948141177433</v>
+        <v>0.9892258576821583</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1026,13 +1038,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>69.29576270641459</v>
+        <v>69.63172944049971</v>
       </c>
       <c r="C26">
-        <v>-0.009161592811863128</v>
+        <v>-0.01405431224028719</v>
       </c>
       <c r="D26">
-        <v>0.7603646063075892</v>
+        <v>0.7799775292504429</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1040,13 +1052,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>69.4014207175926</v>
+        <v>69.95035354970743</v>
       </c>
       <c r="C27">
-        <v>-0.01070030171251357</v>
+        <v>-0.01869446917049644</v>
       </c>
       <c r="D27">
-        <v>0.8414301180748681</v>
+        <v>0.9682743233778685</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1054,13 +1066,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>69.43870492553538</v>
+        <v>70.08798351537729</v>
       </c>
       <c r="C28">
-        <v>-0.01124327561459282</v>
+        <v>-0.02069878905889255</v>
       </c>
       <c r="D28">
-        <v>0.1905261331104081</v>
+        <v>0.6286979954006675</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1068,13 +1080,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>69.49492632348415</v>
+        <v>70.31260923986555</v>
       </c>
       <c r="C29">
-        <v>-0.01206203383714777</v>
+        <v>-0.02397003747377013</v>
       </c>
       <c r="D29">
-        <v>0.7746368177935687</v>
+        <v>0.3296688189892799</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1082,13 +1094,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>69.52444444444444</v>
+        <v>70.6187947275609</v>
       </c>
       <c r="C30">
-        <v>-0.01249190938511324</v>
+        <v>-0.02842904943049862</v>
       </c>
       <c r="D30">
-        <v>0.6236016744899164</v>
+        <v>0.6793822764769371</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1096,13 +1108,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>69.67940033819198</v>
+        <v>71.04033578897823</v>
       </c>
       <c r="C31">
-        <v>-0.0147485486144463</v>
+        <v>-0.03456799692686752</v>
       </c>
       <c r="D31">
-        <v>0.4283953175990722</v>
+        <v>0.4159834639531803</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1110,13 +1122,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>69.70817097949312</v>
+        <v>71.33633125236945</v>
       </c>
       <c r="C32">
-        <v>-0.0151675385363077</v>
+        <v>-0.03887861047139962</v>
       </c>
       <c r="D32">
-        <v>0.3686467433398763</v>
+        <v>0.1960346712108103</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1124,13 +1136,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>69.75474949751715</v>
+        <v>71.3619290845639</v>
       </c>
       <c r="C33">
-        <v>-0.01584586646869646</v>
+        <v>-0.03925139443539671</v>
       </c>
       <c r="D33">
-        <v>0.3920951187367611</v>
+        <v>0.2496007790824726</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1138,13 +1150,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>69.81313689164176</v>
+        <v>71.40240718006947</v>
       </c>
       <c r="C34">
-        <v>-0.01669616832488008</v>
+        <v>-0.03984088126314766</v>
       </c>
       <c r="D34">
-        <v>0.177305120453294</v>
+        <v>0.1959976510120275</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1152,13 +1164,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>69.81794705229312</v>
+        <v>72.49880507734613</v>
       </c>
       <c r="C35">
-        <v>-0.01676621920815213</v>
+        <v>-0.05580784093222513</v>
       </c>
       <c r="D35">
-        <v>0.5869412449801856</v>
+        <v>0.375825839282239</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1166,13 +1178,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>69.92830605712896</v>
+        <v>72.56984439367217</v>
       </c>
       <c r="C36">
-        <v>-0.01837338918148967</v>
+        <v>-0.05684239408260439</v>
       </c>
       <c r="D36">
-        <v>0.2217609132382564</v>
+        <v>0.8605415835064998</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1180,13 +1192,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>70.05367045103949</v>
+        <v>72.67946121561495</v>
       </c>
       <c r="C37">
-        <v>-0.02019908423843919</v>
+        <v>-0.05843875556720812</v>
       </c>
       <c r="D37">
-        <v>0.3742133024092956</v>
+        <v>0.7237012369485465</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1194,13 +1206,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>70.08798351537729</v>
+        <v>72.95297119272102</v>
       </c>
       <c r="C38">
-        <v>-0.02069878905889255</v>
+        <v>-0.06242191057360724</v>
       </c>
       <c r="D38">
-        <v>0.6286979954006675</v>
+        <v>0.5338984762797233</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1208,13 +1220,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>70.11417455559075</v>
+        <v>72.98510130302596</v>
       </c>
       <c r="C39">
-        <v>-0.02108021197462273</v>
+        <v>-0.06288982480134897</v>
       </c>
       <c r="D39">
-        <v>0.6480077540803749</v>
+        <v>0.673749485002807</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1222,13 +1234,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>70.53758752807504</v>
+        <v>73.19876592636992</v>
       </c>
       <c r="C40">
-        <v>-0.02724642031177238</v>
+        <v>-0.06600144552965892</v>
       </c>
       <c r="D40">
-        <v>0.263165033140478</v>
+        <v>0.335690558149955</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1236,13 +1248,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>70.58896874392346</v>
+        <v>73.23004234417333</v>
       </c>
       <c r="C41">
-        <v>-0.0279946904454873</v>
+        <v>-0.06645692734232989</v>
       </c>
       <c r="D41">
-        <v>0.630717229552705</v>
+        <v>0.4684213108442773</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1250,13 +1262,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>70.6187947275609</v>
+        <v>73.27470073630055</v>
       </c>
       <c r="C42">
-        <v>-0.02842904943049862</v>
+        <v>-0.0671072922762217</v>
       </c>
       <c r="D42">
-        <v>0.6793822764769371</v>
+        <v>0.2719754607147543</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1264,13 +1276,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>70.70361771739051</v>
+        <v>73.28897946800609</v>
       </c>
       <c r="C43">
-        <v>-0.02966433569015314</v>
+        <v>-0.06731523497096248</v>
       </c>
       <c r="D43">
-        <v>0.690706519646357</v>
+        <v>0.1073027660341776</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1278,13 +1290,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>70.71944908658377</v>
+        <v>73.73939118020469</v>
       </c>
       <c r="C44">
-        <v>-0.02989488961044318</v>
+        <v>-0.07387462883793239</v>
       </c>
       <c r="D44">
-        <v>0.208245058803033</v>
+        <v>0.8316223179612197</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1292,13 +1304,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>70.77803182557615</v>
+        <v>73.8824357482261</v>
       </c>
       <c r="C45">
-        <v>-0.03074803629479828</v>
+        <v>-0.07595780215863246</v>
       </c>
       <c r="D45">
-        <v>0.5401172483137908</v>
+        <v>0.7108375472717526</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1306,13 +1318,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>70.90300954499139</v>
+        <v>73.97096727693078</v>
       </c>
       <c r="C46">
-        <v>-0.03256810016977751</v>
+        <v>-0.07724709626598214</v>
       </c>
       <c r="D46">
-        <v>0.5498933674778936</v>
+        <v>0.4489121563606467</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1320,13 +1332,13 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>71.57286077106714</v>
+        <v>73.98680982040712</v>
       </c>
       <c r="C47">
-        <v>-0.04232321511262827</v>
+        <v>-0.07747781291855027</v>
       </c>
       <c r="D47">
-        <v>0.828713862852176</v>
+        <v>0.544954115622301</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1334,13 +1346,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>72.67946121561495</v>
+        <v>74.07872152842315</v>
       </c>
       <c r="C48">
-        <v>-0.05843875556720812</v>
+        <v>-0.07881633293820101</v>
       </c>
       <c r="D48">
-        <v>0.7237012369485465</v>
+        <v>0.5503741895625895</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1348,13 +1360,13 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>72.95297119272102</v>
+        <v>74.32541788898709</v>
       </c>
       <c r="C49">
-        <v>-0.06242191057360724</v>
+        <v>-0.08240899838330717</v>
       </c>
       <c r="D49">
-        <v>0.5338984762797233</v>
+        <v>0.7302921781017575</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1362,13 +1374,13 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>72.98510130302596</v>
+        <v>74.4712317275054</v>
       </c>
       <c r="C50">
-        <v>-0.06288982480134897</v>
+        <v>-0.08453250088600095</v>
       </c>
       <c r="D50">
-        <v>0.673749485002807</v>
+        <v>0.5352360565990314</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1376,13 +1388,13 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>73.33692616317538</v>
+        <v>75.02918572413678</v>
       </c>
       <c r="C51">
-        <v>-0.06801348781323369</v>
+        <v>-0.09265804452626392</v>
       </c>
       <c r="D51">
-        <v>0.1162654655903982</v>
+        <v>0.3552493566402254</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1390,13 +1402,13 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>73.97096727693078</v>
+        <v>75.44459093855475</v>
       </c>
       <c r="C52">
-        <v>-0.07724709626598214</v>
+        <v>-0.09870763502749624</v>
       </c>
       <c r="D52">
-        <v>0.4489121563606467</v>
+        <v>0.8530518117283539</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1404,13 +1416,13 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>74.07872152842315</v>
+        <v>76.01117738575996</v>
       </c>
       <c r="C53">
-        <v>-0.07881633293820101</v>
+        <v>-0.1069588939673782</v>
       </c>
       <c r="D53">
-        <v>0.5503741895625895</v>
+        <v>0.08354894275658545</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1418,13 +1430,13 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>74.4712317275054</v>
+        <v>76.0526505767467</v>
       </c>
       <c r="C54">
-        <v>-0.08453250088600095</v>
+        <v>-0.1075628724768938</v>
       </c>
       <c r="D54">
-        <v>0.5352360565990314</v>
+        <v>0.592923696531395</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1432,13 +1444,13 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>75.44459093855475</v>
+        <v>76.25686568806381</v>
       </c>
       <c r="C55">
-        <v>-0.09870763502749624</v>
+        <v>-0.1105368789523857</v>
       </c>
       <c r="D55">
-        <v>0.8530518117283539</v>
+        <v>0.6008581648793865</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1446,13 +1458,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>76.0526505767467</v>
+        <v>76.41352091643235</v>
       </c>
       <c r="C56">
-        <v>-0.1075628724768938</v>
+        <v>-0.1128182657732866</v>
       </c>
       <c r="D56">
-        <v>0.592923696531395</v>
+        <v>0.6832995028492446</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1460,13 +1472,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>76.25686568806381</v>
+        <v>76.48481935503997</v>
       </c>
       <c r="C57">
-        <v>-0.1105368789523857</v>
+        <v>-0.1138565925491257</v>
       </c>
       <c r="D57">
-        <v>0.6008581648793865</v>
+        <v>0.2569171209875381</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1474,13 +1486,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>76.41352091643235</v>
+        <v>76.58789564113016</v>
       </c>
       <c r="C58">
-        <v>-0.1128182657732866</v>
+        <v>-0.1153577035116045</v>
       </c>
       <c r="D58">
-        <v>0.6832995028492446</v>
+        <v>0.3270051834274512</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1488,13 +1500,13 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>77.40325843313184</v>
+        <v>78.04832652780568</v>
       </c>
       <c r="C59">
-        <v>-0.1272319189291045</v>
+        <v>-0.1366261144826071</v>
       </c>
       <c r="D59">
-        <v>0.8828158886126793</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1502,13 +1514,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>78.04832652780568</v>
+        <v>78.42044504162075</v>
       </c>
       <c r="C60">
-        <v>-0.1366261144826071</v>
+        <v>-0.1420453161401081</v>
       </c>
       <c r="D60">
-        <v>0.1993894770059438</v>
+        <v>0.6585534943209588</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1516,13 +1528,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>78.42044504162075</v>
+        <v>78.77084543079066</v>
       </c>
       <c r="C61">
-        <v>-0.1420453161401081</v>
+        <v>-0.1471482344289903</v>
       </c>
       <c r="D61">
-        <v>0.6585534943209588</v>
+        <v>0.3845328308190412</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1530,13 +1542,13 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>78.77084543079066</v>
+        <v>78.88716652562987</v>
       </c>
       <c r="C62">
-        <v>-0.1471482344289903</v>
+        <v>-0.1488422309557746</v>
       </c>
       <c r="D62">
-        <v>0.3845328308190412</v>
+        <v>0.6771909774942169</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1558,13 +1570,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>80.36744132269627</v>
+        <v>81.54008303328142</v>
       </c>
       <c r="C64">
-        <v>-0.1703996309130524</v>
+        <v>-0.1874769373778848</v>
       </c>
       <c r="D64">
-        <v>0.3793736447961062</v>
+        <v>0.460946600399661</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1572,13 +1584,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>81.54008303328142</v>
+        <v>82.16410519655304</v>
       </c>
       <c r="C65">
-        <v>-0.1874769373778848</v>
+        <v>-0.1965646387847528</v>
       </c>
       <c r="D65">
-        <v>0.460946600399661</v>
+        <v>0.6669403734719173</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1586,13 +1598,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>82.16410519655304</v>
+        <v>82.42737389252838</v>
       </c>
       <c r="C66">
-        <v>-0.1965646387847528</v>
+        <v>-0.2003986489203162</v>
       </c>
       <c r="D66">
-        <v>0.6669403734719173</v>
+        <v>0.5677218938123787</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1600,13 +1612,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>82.28188680064255</v>
+        <v>83.55197621317319</v>
       </c>
       <c r="C67">
-        <v>-0.1982799048637265</v>
+        <v>-0.2167763526190272</v>
       </c>
       <c r="D67">
-        <v>0.6348989458559258</v>
+        <v>0.04302603784880898</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1614,13 +1626,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>82.42737389252838</v>
+        <v>84.06729107409046</v>
       </c>
       <c r="C68">
-        <v>-0.2003986489203162</v>
+        <v>-0.2242809379721913</v>
       </c>
       <c r="D68">
-        <v>0.5677218938123787</v>
+        <v>0.6373908156705068</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1628,13 +1640,13 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>84.06729107409046</v>
+        <v>84.1298166982407</v>
       </c>
       <c r="C69">
-        <v>-0.2242809379721913</v>
+        <v>-0.2251915053141849</v>
       </c>
       <c r="D69">
-        <v>0.6373908156705068</v>
+        <v>0.9608017755172092</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1670,13 +1682,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>86.76794162237762</v>
+        <v>84.94995814606555</v>
       </c>
       <c r="C72">
-        <v>-0.2636108003258877</v>
+        <v>-0.2371353128067799</v>
       </c>
       <c r="D72">
-        <v>0.4965940057828593</v>
+        <v>0.04114554308726114</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1684,13 +1696,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>86.91429774666446</v>
+        <v>86.76794162237762</v>
       </c>
       <c r="C73">
-        <v>-0.2657422001941427</v>
+        <v>-0.2636108003258877</v>
       </c>
       <c r="D73">
-        <v>0.1575450248366336</v>
+        <v>0.4965940057828593</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1698,13 +1710,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>87.19950236364741</v>
+        <v>86.91429774666446</v>
       </c>
       <c r="C74">
-        <v>-0.2698956654900109</v>
+        <v>-0.2657422001941427</v>
       </c>
       <c r="D74">
-        <v>0.5041128285123215</v>
+        <v>0.1575450248366336</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1712,13 +1724,13 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>87.82892920421926</v>
+        <v>87.19950236364741</v>
       </c>
       <c r="C75">
-        <v>-0.279062075789601</v>
+        <v>-0.2698956654900109</v>
       </c>
       <c r="D75">
-        <v>0.4951587728324055</v>
+        <v>0.5041128285123215</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1726,13 +1738,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>87.87863301108423</v>
+        <v>87.82892920421926</v>
       </c>
       <c r="C76">
-        <v>-0.2797859176371491</v>
+        <v>-0.279062075789601</v>
       </c>
       <c r="D76">
-        <v>0.9010750088292466</v>
+        <v>0.4951587728324055</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1740,13 +1752,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>87.93795344894419</v>
+        <v>87.87863301108423</v>
       </c>
       <c r="C77">
-        <v>-0.2806498075088959</v>
+        <v>-0.2797859176371491</v>
       </c>
       <c r="D77">
-        <v>0.2842208860046075</v>
+        <v>0.9010750088292466</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1754,13 +1766,13 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>89.6919664851593</v>
+        <v>87.93795344894419</v>
       </c>
       <c r="C78">
-        <v>-0.3061936866770774</v>
+        <v>-0.2806498075088959</v>
       </c>
       <c r="D78">
-        <v>0.172934894487245</v>
+        <v>0.2842208860046075</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1768,13 +1780,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>90.13564128700503</v>
+        <v>89.6919664851593</v>
       </c>
       <c r="C79">
-        <v>-0.3126549701991024</v>
+        <v>-0.3061936866770774</v>
       </c>
       <c r="D79">
-        <v>0.4797436354169866</v>
+        <v>0.172934894487245</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1782,13 +1794,13 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>92.06308817163205</v>
+        <v>89.78170132535439</v>
       </c>
       <c r="C80">
-        <v>-0.3407245850237675</v>
+        <v>-0.3075005047381707</v>
       </c>
       <c r="D80">
-        <v>0.3592600093145459</v>
+        <v>0.9936400395210836</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1796,13 +1808,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>92.19602611535281</v>
+        <v>90.13564128700503</v>
       </c>
       <c r="C81">
-        <v>-0.3426605744954292</v>
+        <v>-0.3126549701991024</v>
       </c>
       <c r="D81">
-        <v>0.3644452569697556</v>
+        <v>0.4797436354169866</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1810,13 +1822,13 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>92.20445228328354</v>
+        <v>92.06308817163205</v>
       </c>
       <c r="C82">
-        <v>-0.3427832856788866</v>
+        <v>-0.3407245850237675</v>
       </c>
       <c r="D82">
-        <v>0.4619489869600593</v>
+        <v>0.3592600093145459</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1824,13 +1836,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>92.76578542452691</v>
+        <v>92.19602611535281</v>
       </c>
       <c r="C83">
-        <v>-0.3509580401630132</v>
+        <v>-0.3426605744954292</v>
       </c>
       <c r="D83">
-        <v>0.3049588857678167</v>
+        <v>0.3644452569697556</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1838,13 +1850,13 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>93.95962765462004</v>
+        <v>92.20445228328354</v>
       </c>
       <c r="C84">
-        <v>-0.3683440920575733</v>
+        <v>-0.3427832856788866</v>
       </c>
       <c r="D84">
-        <v>0.2734771799881525</v>
+        <v>0.4619489869600593</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1852,13 +1864,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>94.75653076747105</v>
+        <v>92.76578542452691</v>
       </c>
       <c r="C85">
-        <v>-0.3799494771961804</v>
+        <v>-0.3509580401630132</v>
       </c>
       <c r="D85">
-        <v>0.525151115091694</v>
+        <v>0.3049588857678167</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1866,13 +1878,13 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>95.77136889358938</v>
+        <v>93.95962765462004</v>
       </c>
       <c r="C86">
-        <v>-0.3947286732076123</v>
+        <v>-0.3683440920575733</v>
       </c>
       <c r="D86">
-        <v>0.2057368121729404</v>
+        <v>0.2734771799881525</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1880,13 +1892,13 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>96.41666666666667</v>
+        <v>94.75653076747105</v>
       </c>
       <c r="C87">
-        <v>-0.404126213592233</v>
+        <v>-0.3799494771961804</v>
       </c>
       <c r="D87">
-        <v>0.7177442608848796</v>
+        <v>0.525151115091694</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1894,13 +1906,13 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>98.99833579341056</v>
+        <v>95.77136889358938</v>
       </c>
       <c r="C88">
-        <v>-0.4417233367972411</v>
+        <v>-0.3947286732076123</v>
       </c>
       <c r="D88">
-        <v>0.1230859775533545</v>
+        <v>0.2057368121729404</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1908,13 +1920,13 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>99.32189611486321</v>
+        <v>98.99833579341056</v>
       </c>
       <c r="C89">
-        <v>-0.4464353803135419</v>
+        <v>-0.4417233367972411</v>
       </c>
       <c r="D89">
-        <v>0.7968291490643427</v>
+        <v>0.1230859775533545</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1950,13 +1962,13 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>100.9376213475724</v>
+        <v>100.5385274468751</v>
       </c>
       <c r="C92">
-        <v>-0.4699653594306659</v>
+        <v>-0.4641533123331321</v>
       </c>
       <c r="D92">
-        <v>0.1527582076606218</v>
+        <v>0.9966713701571901</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1964,13 +1976,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>101.5943459520473</v>
+        <v>100.9376213475724</v>
       </c>
       <c r="C93">
-        <v>-0.4795293099812712</v>
+        <v>-0.4699653594306659</v>
       </c>
       <c r="D93">
-        <v>0.3665338245643951</v>
+        <v>0.1527582076606218</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1978,13 +1990,13 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>104.6524401869776</v>
+        <v>101.5943459520473</v>
       </c>
       <c r="C94">
-        <v>-0.5240646629171493</v>
+        <v>-0.4795293099812712</v>
       </c>
       <c r="D94">
-        <v>0.2559735297086234</v>
+        <v>0.3665338245643951</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1992,13 +2004,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>106.1667400085034</v>
+        <v>104.6524401869776</v>
       </c>
       <c r="C95">
-        <v>-0.5461175729393697</v>
+        <v>-0.5240646629171493</v>
       </c>
       <c r="D95">
-        <v>0.09131726118289579</v>
+        <v>0.2559735297086234</v>
       </c>
     </row>
     <row r="96" spans="1:4">

</xml_diff>

<commit_message>
Backup: Wed Jan  1 18:20:23 IST 2025
</commit_message>
<xml_diff>
--- a/linear_regression_with_significance.xlsx
+++ b/linear_regression_with_significance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>Feature</t>
   </si>
@@ -28,298 +28,442 @@
     <t>P-value</t>
   </si>
   <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Pole Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Frontal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
+  </si>
+  <si>
     <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
   </si>
   <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age at baseline </t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
     <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
   </si>
   <si>
-    <t>Temporal Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
+    <t>Frontal Medial Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Change</t>
   </si>
   <si>
     <t>Parahippocampal Gyrus, anterior division Volume Change</t>
   </si>
   <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age at baseline </t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
+    <t>Frontal Opercular Cortex Volume Avg</t>
   </si>
   <si>
     <t>Cingulate Gyrus, anterior division Change</t>
   </si>
   <si>
-    <t>Supramarginal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Change</t>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Avg</t>
   </si>
 </sst>
 </file>
@@ -677,7 +821,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -702,13 +846,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>39.6969084606372</v>
+        <v>66.59423698792997</v>
       </c>
       <c r="C2">
-        <v>0.4218896826120796</v>
+        <v>0.03018101473888379</v>
       </c>
       <c r="D2">
-        <v>0.01327284346805847</v>
+        <v>0.06642380016329742</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -716,13 +860,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>61.86812217071104</v>
+        <v>68.16138662459012</v>
       </c>
       <c r="C3">
-        <v>0.09900792955275184</v>
+        <v>0.007358447214706909</v>
       </c>
       <c r="D3">
-        <v>0.1676739325884186</v>
+        <v>0.1097106966731553</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -730,13 +874,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>66.12200276610442</v>
+        <v>68.17881946219434</v>
       </c>
       <c r="C4">
-        <v>0.03705821214411043</v>
+        <v>0.007104570938917254</v>
       </c>
       <c r="D4">
-        <v>0.09346911303928794</v>
+        <v>0.08480979062589011</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -744,13 +888,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>66.98652591476593</v>
+        <v>68.52473897014218</v>
       </c>
       <c r="C5">
-        <v>0.02446806920243783</v>
+        <v>0.002066908201812989</v>
       </c>
       <c r="D5">
-        <v>0.4556668748933871</v>
+        <v>0.3341296243439147</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -758,13 +902,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>67.64606448730302</v>
+        <v>68.75213069530646</v>
       </c>
       <c r="C6">
-        <v>0.01486313853442212</v>
+        <v>-0.001244621776307797</v>
       </c>
       <c r="D6">
-        <v>0.4604050421945982</v>
+        <v>0.3909978602464819</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -772,13 +916,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>67.8513832008049</v>
+        <v>68.85444444444445</v>
       </c>
       <c r="C7">
-        <v>0.01187306018245293</v>
+        <v>-0.002734627831715297</v>
       </c>
       <c r="D7">
-        <v>0.4956594214689176</v>
+        <v>0.7220787472790002</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -786,13 +930,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>68.07909947890576</v>
+        <v>69.24741001944062</v>
       </c>
       <c r="C8">
-        <v>0.008556803705255911</v>
+        <v>-0.008457427467581935</v>
       </c>
       <c r="D8">
-        <v>0.06318905803758798</v>
+        <v>0.07650593831687533</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -800,13 +944,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>68.48992841584712</v>
+        <v>69.27549839102056</v>
       </c>
       <c r="C9">
-        <v>0.002573858021644004</v>
+        <v>-0.00886648142262958</v>
       </c>
       <c r="D9">
-        <v>0.3186013917789818</v>
+        <v>0.07093315664320629</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -814,13 +958,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>68.66766388657908</v>
+        <v>69.29553967652757</v>
       </c>
       <c r="C10">
-        <v>-1.452262008383443E-05</v>
+        <v>-0.009158344803799512</v>
       </c>
       <c r="D10">
-        <v>0.2675875235013904</v>
+        <v>0.4391528556590062</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -828,13 +972,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>68.85444444444445</v>
+        <v>69.30366624678693</v>
       </c>
       <c r="C11">
-        <v>-0.002734627831715297</v>
+        <v>-0.009276692914372831</v>
       </c>
       <c r="D11">
-        <v>0.7220787472790002</v>
+        <v>0.3271322762958427</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -842,13 +986,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>68.90581617919213</v>
+        <v>69.33243864201874</v>
       </c>
       <c r="C12">
-        <v>-0.003482759891147547</v>
+        <v>-0.009695708378913759</v>
       </c>
       <c r="D12">
-        <v>0.7303388057829046</v>
+        <v>0.4941094742326387</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -856,13 +1000,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>69.01826504146955</v>
+        <v>69.37661450970899</v>
       </c>
       <c r="C13">
-        <v>-0.00512036468159538</v>
+        <v>-0.01033904625789783</v>
       </c>
       <c r="D13">
-        <v>0.4031055848774701</v>
+        <v>0.2417817650283086</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -870,13 +1014,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>69.06355495859624</v>
+        <v>69.59263347285057</v>
       </c>
       <c r="C14">
-        <v>-0.005779926581498618</v>
+        <v>-0.01348495348811518</v>
       </c>
       <c r="D14">
-        <v>0.2040618196925583</v>
+        <v>0.6762567704008368</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -884,13 +1028,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>69.10255892610388</v>
+        <v>69.63725407650463</v>
       </c>
       <c r="C15">
-        <v>-0.006347945525784882</v>
+        <v>-0.01413476810443637</v>
       </c>
       <c r="D15">
-        <v>0.3340370223553067</v>
+        <v>0.6689881118953149</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -898,13 +1042,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>69.13824000939569</v>
+        <v>69.71068687095443</v>
       </c>
       <c r="C16">
-        <v>-0.006867572952364398</v>
+        <v>-0.01520417773234617</v>
       </c>
       <c r="D16">
-        <v>0.5565832971759981</v>
+        <v>0.9612333186185186</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -912,13 +1056,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>69.14638220513085</v>
+        <v>69.71812660629979</v>
       </c>
       <c r="C17">
-        <v>-0.006986148618410404</v>
+        <v>-0.01531252339271538</v>
       </c>
       <c r="D17">
-        <v>0.4569685920449683</v>
+        <v>0.7543409199568036</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -926,13 +1070,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>69.2027704034229</v>
+        <v>69.89083403266828</v>
       </c>
       <c r="C18">
-        <v>-0.007807335972178198</v>
+        <v>-0.01782768008740221</v>
       </c>
       <c r="D18">
-        <v>0.4487351500627458</v>
+        <v>0.9042531239699123</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -940,13 +1084,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>69.22075130267341</v>
+        <v>70.10954834481979</v>
       </c>
       <c r="C19">
-        <v>-0.008069193728253543</v>
+        <v>-0.02101283997310377</v>
       </c>
       <c r="D19">
-        <v>0.9477832899558639</v>
+        <v>0.3496185694580984</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -954,13 +1098,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>69.24781957267116</v>
+        <v>70.13095865292946</v>
       </c>
       <c r="C20">
-        <v>-0.008463391835016765</v>
+        <v>-0.02132464057664274</v>
       </c>
       <c r="D20">
-        <v>0.766764388878391</v>
+        <v>0.3718261415270548</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -968,13 +1112,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>69.26387073719739</v>
+        <v>70.63313944237514</v>
       </c>
       <c r="C21">
-        <v>-0.008697146658214416</v>
+        <v>-0.02863795304429817</v>
       </c>
       <c r="D21">
-        <v>0.5094561817189306</v>
+        <v>0.3917971852357461</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -982,13 +1126,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>69.31002826128042</v>
+        <v>70.68300303261805</v>
       </c>
       <c r="C22">
-        <v>-0.009369343610879932</v>
+        <v>-0.02936412183424331</v>
       </c>
       <c r="D22">
-        <v>0.9494539888673468</v>
+        <v>0.5877898348980366</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -996,13 +1140,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>69.56447608405639</v>
+        <v>70.91788020411116</v>
       </c>
       <c r="C23">
-        <v>-0.01307489442800569</v>
+        <v>-0.03278466316666728</v>
       </c>
       <c r="D23">
-        <v>0.08599038957451426</v>
+        <v>0.8301695072308871</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1010,13 +1154,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>69.56874263372083</v>
+        <v>70.94279226951211</v>
       </c>
       <c r="C24">
-        <v>-0.01313702864641986</v>
+        <v>-0.03314746023561321</v>
       </c>
       <c r="D24">
-        <v>0.9619947627823591</v>
+        <v>0.3162590352277476</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1024,13 +1168,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>69.57062689014457</v>
+        <v>71.4781022415147</v>
       </c>
       <c r="C25">
-        <v>-0.0131644692739501</v>
+        <v>-0.04094323652691334</v>
       </c>
       <c r="D25">
-        <v>0.9892258576821583</v>
+        <v>0.2509792573418467</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1038,13 +1182,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>69.63172944049971</v>
+        <v>71.64196197132816</v>
       </c>
       <c r="C26">
-        <v>-0.01405431224028719</v>
+        <v>-0.0433295432717693</v>
       </c>
       <c r="D26">
-        <v>0.7799775292504429</v>
+        <v>0.6011361304583829</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1052,13 +1196,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>69.95035354970743</v>
+        <v>71.7596823911008</v>
       </c>
       <c r="C27">
-        <v>-0.01869446917049644</v>
+        <v>-0.04504391831700194</v>
       </c>
       <c r="D27">
-        <v>0.9682743233778685</v>
+        <v>0.7370905313725307</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1066,13 +1210,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>70.08798351537729</v>
+        <v>71.77249003998783</v>
       </c>
       <c r="C28">
-        <v>-0.02069878905889255</v>
+        <v>-0.045230437475551</v>
       </c>
       <c r="D28">
-        <v>0.6286979954006675</v>
+        <v>0.2048030899584639</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1080,13 +1224,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>70.31260923986555</v>
+        <v>71.78485382574682</v>
       </c>
       <c r="C29">
-        <v>-0.02397003747377013</v>
+        <v>-0.04541049260796348</v>
       </c>
       <c r="D29">
-        <v>0.3296688189892799</v>
+        <v>0.7540364712875921</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1094,13 +1238,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>70.6187947275609</v>
+        <v>71.91310317051254</v>
       </c>
       <c r="C30">
-        <v>-0.02842904943049862</v>
+        <v>-0.04727820151231854</v>
       </c>
       <c r="D30">
-        <v>0.6793822764769371</v>
+        <v>0.4160962829806277</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1108,13 +1252,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>71.04033578897823</v>
+        <v>72.00679428291419</v>
       </c>
       <c r="C31">
-        <v>-0.03456799692686752</v>
+        <v>-0.04864263518807066</v>
       </c>
       <c r="D31">
-        <v>0.4159834639531803</v>
+        <v>0.2503233825440773</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1122,13 +1266,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>71.33633125236945</v>
+        <v>72.03111111973122</v>
       </c>
       <c r="C32">
-        <v>-0.03887861047139962</v>
+        <v>-0.04899676387958096</v>
       </c>
       <c r="D32">
-        <v>0.1960346712108103</v>
+        <v>0.4776474817936434</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1136,13 +1280,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>71.3619290845639</v>
+        <v>72.0610489185684</v>
       </c>
       <c r="C33">
-        <v>-0.03925139443539671</v>
+        <v>-0.04943275124128754</v>
       </c>
       <c r="D33">
-        <v>0.2496007790824726</v>
+        <v>0.2576322561943097</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1150,13 +1294,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>71.40240718006947</v>
+        <v>72.07231866221065</v>
       </c>
       <c r="C34">
-        <v>-0.03984088126314766</v>
+        <v>-0.04959687372151422</v>
       </c>
       <c r="D34">
-        <v>0.1959976510120275</v>
+        <v>0.8237748274183451</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1164,13 +1308,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>72.49880507734613</v>
+        <v>72.09938088727624</v>
       </c>
       <c r="C35">
-        <v>-0.05580784093222513</v>
+        <v>-0.04999098379528499</v>
       </c>
       <c r="D35">
-        <v>0.375825839282239</v>
+        <v>0.3914827555738817</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1178,13 +1322,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>72.56984439367217</v>
+        <v>72.37802672217569</v>
       </c>
       <c r="C36">
-        <v>-0.05684239408260439</v>
+        <v>-0.0540489328472189</v>
       </c>
       <c r="D36">
-        <v>0.8605415835064998</v>
+        <v>0.2494410519063999</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1192,13 +1336,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>72.67946121561495</v>
+        <v>72.41757893873393</v>
       </c>
       <c r="C37">
-        <v>-0.05843875556720812</v>
+        <v>-0.0546249360009794</v>
       </c>
       <c r="D37">
-        <v>0.7237012369485465</v>
+        <v>0.508645371357745</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1206,13 +1350,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>72.95297119272102</v>
+        <v>72.42061271392267</v>
       </c>
       <c r="C38">
-        <v>-0.06242191057360724</v>
+        <v>-0.05466911719304846</v>
       </c>
       <c r="D38">
-        <v>0.5338984762797233</v>
+        <v>0.3628264964311102</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1220,13 +1364,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>72.98510130302596</v>
+        <v>72.54908992736631</v>
       </c>
       <c r="C39">
-        <v>-0.06288982480134897</v>
+        <v>-0.05654014457329581</v>
       </c>
       <c r="D39">
-        <v>0.673749485002807</v>
+        <v>0.1565635495080199</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1234,13 +1378,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>73.19876592636992</v>
+        <v>72.60533162098335</v>
       </c>
       <c r="C40">
-        <v>-0.06600144552965892</v>
+        <v>-0.0573591983638353</v>
       </c>
       <c r="D40">
-        <v>0.335690558149955</v>
+        <v>0.4231977165777575</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1248,13 +1392,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>73.23004234417333</v>
+        <v>72.64792032050312</v>
       </c>
       <c r="C41">
-        <v>-0.06645692734232989</v>
+        <v>-0.05797942214324925</v>
       </c>
       <c r="D41">
-        <v>0.4684213108442773</v>
+        <v>0.9463965949281148</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1262,13 +1406,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>73.27470073630055</v>
+        <v>72.70359741803151</v>
       </c>
       <c r="C42">
-        <v>-0.0671072922762217</v>
+        <v>-0.05879025366065282</v>
       </c>
       <c r="D42">
-        <v>0.2719754607147543</v>
+        <v>0.3401954873152755</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1276,13 +1420,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>73.28897946800609</v>
+        <v>73.07051795899049</v>
       </c>
       <c r="C43">
-        <v>-0.06731523497096248</v>
+        <v>-0.06413375668432764</v>
       </c>
       <c r="D43">
-        <v>0.1073027660341776</v>
+        <v>0.9143159910348685</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1290,13 +1434,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>73.73939118020469</v>
+        <v>73.07173612519739</v>
       </c>
       <c r="C44">
-        <v>-0.07387462883793239</v>
+        <v>-0.06415149696889411</v>
       </c>
       <c r="D44">
-        <v>0.8316223179612197</v>
+        <v>0.5471063243532105</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1304,13 +1448,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>73.8824357482261</v>
+        <v>73.42682227697128</v>
       </c>
       <c r="C45">
-        <v>-0.07595780215863246</v>
+        <v>-0.06932265451899911</v>
       </c>
       <c r="D45">
-        <v>0.7108375472717526</v>
+        <v>0.665450348860845</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1318,13 +1462,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>73.97096727693078</v>
+        <v>73.48171565862555</v>
       </c>
       <c r="C46">
-        <v>-0.07724709626598214</v>
+        <v>-0.07012207269843018</v>
       </c>
       <c r="D46">
-        <v>0.4489121563606467</v>
+        <v>0.3843044519508477</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1332,13 +1476,13 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>73.98680982040712</v>
+        <v>73.50065569481541</v>
       </c>
       <c r="C47">
-        <v>-0.07747781291855027</v>
+        <v>-0.07039789846818545</v>
       </c>
       <c r="D47">
-        <v>0.544954115622301</v>
+        <v>0.5174898701146766</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1346,13 +1490,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>74.07872152842315</v>
+        <v>73.54150900529288</v>
       </c>
       <c r="C48">
-        <v>-0.07881633293820101</v>
+        <v>-0.07099284959164409</v>
       </c>
       <c r="D48">
-        <v>0.5503741895625895</v>
+        <v>0.3360406024248999</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1360,13 +1504,13 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>74.32541788898709</v>
+        <v>73.56392282811139</v>
       </c>
       <c r="C49">
-        <v>-0.08240899838330717</v>
+        <v>-0.07131926448705905</v>
       </c>
       <c r="D49">
-        <v>0.7302921781017575</v>
+        <v>0.8548880351145752</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1374,13 +1518,13 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>74.4712317275054</v>
+        <v>73.98103206003272</v>
       </c>
       <c r="C50">
-        <v>-0.08453250088600095</v>
+        <v>-0.07739367077717541</v>
       </c>
       <c r="D50">
-        <v>0.5352360565990314</v>
+        <v>0.5063429355965893</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1388,13 +1532,13 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>75.02918572413678</v>
+        <v>74.00237266091189</v>
       </c>
       <c r="C51">
-        <v>-0.09265804452626392</v>
+        <v>-0.07770445622687205</v>
       </c>
       <c r="D51">
-        <v>0.3552493566402254</v>
+        <v>0.4590559345945862</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1402,13 +1546,13 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>75.44459093855475</v>
+        <v>74.27877753086949</v>
       </c>
       <c r="C52">
-        <v>-0.09870763502749624</v>
+        <v>-0.0817297698670314</v>
       </c>
       <c r="D52">
-        <v>0.8530518117283539</v>
+        <v>0.2808363772281603</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1416,13 +1560,13 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>76.01117738575996</v>
+        <v>74.43885136592287</v>
       </c>
       <c r="C53">
-        <v>-0.1069588939673782</v>
+        <v>-0.08406094222217786</v>
       </c>
       <c r="D53">
-        <v>0.08354894275658545</v>
+        <v>0.3168781560213524</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1430,13 +1574,13 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>76.0526505767467</v>
+        <v>74.60912715707212</v>
       </c>
       <c r="C54">
-        <v>-0.1075628724768938</v>
+        <v>-0.08654068675347748</v>
       </c>
       <c r="D54">
-        <v>0.592923696531395</v>
+        <v>0.1006035393123007</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1444,13 +1588,13 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>76.25686568806381</v>
+        <v>74.64077675366418</v>
       </c>
       <c r="C55">
-        <v>-0.1105368789523857</v>
+        <v>-0.08700160320870176</v>
       </c>
       <c r="D55">
-        <v>0.6008581648793865</v>
+        <v>0.6602933186327933</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1458,13 +1602,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>76.41352091643235</v>
+        <v>74.66872975976717</v>
       </c>
       <c r="C56">
-        <v>-0.1128182657732866</v>
+        <v>-0.08740868582185213</v>
       </c>
       <c r="D56">
-        <v>0.6832995028492446</v>
+        <v>0.1181700061233251</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1472,13 +1616,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>76.48481935503997</v>
+        <v>74.80688010552694</v>
       </c>
       <c r="C57">
-        <v>-0.1138565925491257</v>
+        <v>-0.08942058406107201</v>
       </c>
       <c r="D57">
-        <v>0.2569171209875381</v>
+        <v>0.2712948357901225</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1486,13 +1630,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>76.58789564113016</v>
+        <v>74.84424102580176</v>
       </c>
       <c r="C58">
-        <v>-0.1153577035116045</v>
+        <v>-0.08996467513303541</v>
       </c>
       <c r="D58">
-        <v>0.3270051834274512</v>
+        <v>0.8751993739755017</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1500,13 +1644,13 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>78.04832652780568</v>
+        <v>74.96469212605746</v>
       </c>
       <c r="C59">
-        <v>-0.1366261144826071</v>
+        <v>-0.09171881736976872</v>
       </c>
       <c r="D59">
-        <v>0.1993894770059438</v>
+        <v>0.2883749869531166</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1514,13 +1658,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>78.42044504162075</v>
+        <v>74.96476981534681</v>
       </c>
       <c r="C60">
-        <v>-0.1420453161401081</v>
+        <v>-0.0917199487671867</v>
       </c>
       <c r="D60">
-        <v>0.6585534943209588</v>
+        <v>0.2581464690080968</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1528,13 +1672,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>78.77084543079066</v>
+        <v>75.03923748539688</v>
       </c>
       <c r="C61">
-        <v>-0.1471482344289903</v>
+        <v>-0.09280442939898359</v>
       </c>
       <c r="D61">
-        <v>0.3845328308190412</v>
+        <v>0.2579348610750429</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1542,13 +1686,13 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>78.88716652562987</v>
+        <v>75.08854297568931</v>
       </c>
       <c r="C62">
-        <v>-0.1488422309557746</v>
+        <v>-0.09352247051974705</v>
       </c>
       <c r="D62">
-        <v>0.6771909774942169</v>
+        <v>0.87152087201016</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1556,13 +1700,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>79.38466530558603</v>
+        <v>75.17714197809377</v>
       </c>
       <c r="C63">
-        <v>-0.156087358819214</v>
+        <v>-0.09481274725379274</v>
       </c>
       <c r="D63">
-        <v>0.5013574565563785</v>
+        <v>0.8965680567360108</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1570,13 +1714,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>81.54008303328142</v>
+        <v>75.23338806505173</v>
       </c>
       <c r="C64">
-        <v>-0.1874769373778848</v>
+        <v>-0.09563186502502519</v>
       </c>
       <c r="D64">
-        <v>0.460946600399661</v>
+        <v>0.9511237536532267</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1584,13 +1728,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>82.16410519655304</v>
+        <v>75.34189074166845</v>
       </c>
       <c r="C65">
-        <v>-0.1965646387847528</v>
+        <v>-0.09721200109225903</v>
       </c>
       <c r="D65">
-        <v>0.6669403734719173</v>
+        <v>0.2402870725843666</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1598,13 +1742,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>82.42737389252838</v>
+        <v>75.46846037999734</v>
       </c>
       <c r="C66">
-        <v>-0.2003986489203162</v>
+        <v>-0.09905524825238854</v>
       </c>
       <c r="D66">
-        <v>0.5677218938123787</v>
+        <v>0.8090353770080231</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1612,13 +1756,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>83.55197621317319</v>
+        <v>75.4840861277309</v>
       </c>
       <c r="C67">
-        <v>-0.2167763526190272</v>
+        <v>-0.09928280768540154</v>
       </c>
       <c r="D67">
-        <v>0.04302603784880898</v>
+        <v>0.3127923493628082</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1626,13 +1770,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>84.06729107409046</v>
+        <v>75.67384357768925</v>
       </c>
       <c r="C68">
-        <v>-0.2242809379721913</v>
+        <v>-0.1020462656945036</v>
       </c>
       <c r="D68">
-        <v>0.6373908156705068</v>
+        <v>0.3727098921061366</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1640,13 +1784,13 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>84.1298166982407</v>
+        <v>75.97598208706351</v>
       </c>
       <c r="C69">
-        <v>-0.2251915053141849</v>
+        <v>-0.1064463410737404</v>
       </c>
       <c r="D69">
-        <v>0.9608017755172092</v>
+        <v>0.5235283678654631</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1654,13 +1798,13 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>84.34221911908804</v>
+        <v>76.14800389417231</v>
       </c>
       <c r="C70">
-        <v>-0.2282847444527385</v>
+        <v>-0.1089515130219267</v>
       </c>
       <c r="D70">
-        <v>0.1999396955676848</v>
+        <v>0.5956900019668596</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1668,13 +1812,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>84.43624278148933</v>
+        <v>76.15965385401753</v>
       </c>
       <c r="C71">
-        <v>-0.2296540210896505</v>
+        <v>-0.1091211726313233</v>
       </c>
       <c r="D71">
-        <v>0.4320966585166013</v>
+        <v>0.1624100038798964</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1682,13 +1826,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>84.94995814606555</v>
+        <v>76.37132679036255</v>
       </c>
       <c r="C72">
-        <v>-0.2371353128067799</v>
+        <v>-0.1122037882091633</v>
       </c>
       <c r="D72">
-        <v>0.04114554308726114</v>
+        <v>0.4366620182425804</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1696,13 +1840,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>86.76794162237762</v>
+        <v>76.40869258796346</v>
       </c>
       <c r="C73">
-        <v>-0.2636108003258877</v>
+        <v>-0.1127479503101476</v>
       </c>
       <c r="D73">
-        <v>0.4965940057828593</v>
+        <v>0.254753596259286</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1710,13 +1854,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>86.91429774666446</v>
+        <v>76.71373262384759</v>
       </c>
       <c r="C74">
-        <v>-0.2657422001941427</v>
+        <v>-0.1171902809298193</v>
       </c>
       <c r="D74">
-        <v>0.1575450248366336</v>
+        <v>0.3064701872772926</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1724,13 +1868,13 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>87.19950236364741</v>
+        <v>76.84343541838646</v>
       </c>
       <c r="C75">
-        <v>-0.2698956654900109</v>
+        <v>-0.1190791565784435</v>
       </c>
       <c r="D75">
-        <v>0.5041128285123215</v>
+        <v>0.0961181785475114</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1738,13 +1882,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>87.82892920421926</v>
+        <v>76.87237573320938</v>
       </c>
       <c r="C76">
-        <v>-0.279062075789601</v>
+        <v>-0.119500617473923</v>
       </c>
       <c r="D76">
-        <v>0.4951587728324055</v>
+        <v>0.3021721792171578</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1752,13 +1896,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>87.87863301108423</v>
+        <v>77.05323264393112</v>
       </c>
       <c r="C77">
-        <v>-0.2797859176371491</v>
+        <v>-0.1221344559795794</v>
       </c>
       <c r="D77">
-        <v>0.9010750088292466</v>
+        <v>0.08379749177553178</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1766,13 +1910,13 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>87.93795344894419</v>
+        <v>77.05630596113535</v>
       </c>
       <c r="C78">
-        <v>-0.2806498075088959</v>
+        <v>-0.1221792130262429</v>
       </c>
       <c r="D78">
-        <v>0.2842208860046075</v>
+        <v>0.1475134422132613</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1780,13 +1924,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>89.6919664851593</v>
+        <v>77.24424857758645</v>
       </c>
       <c r="C79">
-        <v>-0.3061936866770774</v>
+        <v>-0.1249162414211618</v>
       </c>
       <c r="D79">
-        <v>0.172934894487245</v>
+        <v>0.3372964662605143</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1794,13 +1938,13 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>89.78170132535439</v>
+        <v>77.50249451817179</v>
       </c>
       <c r="C80">
-        <v>-0.3075005047381707</v>
+        <v>-0.1286771046335697</v>
       </c>
       <c r="D80">
-        <v>0.9936400395210836</v>
+        <v>0.06160749494133213</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1808,13 +1952,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>90.13564128700503</v>
+        <v>77.52910820784818</v>
       </c>
       <c r="C81">
-        <v>-0.3126549701991024</v>
+        <v>-0.1290646826385657</v>
       </c>
       <c r="D81">
-        <v>0.4797436354169866</v>
+        <v>0.404394464065313</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1822,13 +1966,13 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>92.06308817163205</v>
+        <v>77.7462494641948</v>
       </c>
       <c r="C82">
-        <v>-0.3407245850237675</v>
+        <v>-0.1322269339445845</v>
       </c>
       <c r="D82">
-        <v>0.3592600093145459</v>
+        <v>0.254664207438851</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1836,13 +1980,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>92.19602611535281</v>
+        <v>78.04832652780568</v>
       </c>
       <c r="C83">
-        <v>-0.3426605744954292</v>
+        <v>-0.1366261144826071</v>
       </c>
       <c r="D83">
-        <v>0.3644452569697556</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1850,13 +1994,13 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>92.20445228328354</v>
+        <v>78.16336219751844</v>
       </c>
       <c r="C84">
-        <v>-0.3427832856788866</v>
+        <v>-0.1383013912259967</v>
       </c>
       <c r="D84">
-        <v>0.4619489869600593</v>
+        <v>0.1582330455856755</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1864,13 +2008,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>92.76578542452691</v>
+        <v>78.26990814492322</v>
       </c>
       <c r="C85">
-        <v>-0.3509580401630132</v>
+        <v>-0.1398530312367459</v>
       </c>
       <c r="D85">
-        <v>0.3049588857678167</v>
+        <v>0.4319140410224465</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1878,13 +2022,13 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>93.95962765462004</v>
+        <v>78.33914620546885</v>
       </c>
       <c r="C86">
-        <v>-0.3683440920575733</v>
+        <v>-0.1408613525068279</v>
       </c>
       <c r="D86">
-        <v>0.2734771799881525</v>
+        <v>0.4705476220564199</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1892,13 +2036,13 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>94.75653076747105</v>
+        <v>78.57824052790221</v>
       </c>
       <c r="C87">
-        <v>-0.3799494771961804</v>
+        <v>-0.1443433086587702</v>
       </c>
       <c r="D87">
-        <v>0.525151115091694</v>
+        <v>0.3705359396786212</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1906,13 +2050,13 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>95.77136889358938</v>
+        <v>78.67261287526486</v>
       </c>
       <c r="C88">
-        <v>-0.3947286732076123</v>
+        <v>-0.1457176632320125</v>
       </c>
       <c r="D88">
-        <v>0.2057368121729404</v>
+        <v>0.2210803126090004</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1920,13 +2064,13 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>98.99833579341056</v>
+        <v>78.79633193470507</v>
       </c>
       <c r="C89">
-        <v>-0.4417233367972411</v>
+        <v>-0.1475193971073554</v>
       </c>
       <c r="D89">
-        <v>0.1230859775533545</v>
+        <v>0.06687712153272754</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1934,13 +2078,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>99.46419101294769</v>
+        <v>78.9036459402825</v>
       </c>
       <c r="C90">
-        <v>-0.4485076361108888</v>
+        <v>-0.1490822224312984</v>
       </c>
       <c r="D90">
-        <v>0.2951161971661123</v>
+        <v>0.1673134047190758</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1948,13 +2092,13 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>100.1822894068573</v>
+        <v>78.91968371136763</v>
       </c>
       <c r="C91">
-        <v>-0.4589653797115139</v>
+        <v>-0.1493157822043829</v>
       </c>
       <c r="D91">
-        <v>0.3576237376024517</v>
+        <v>0.3690873343607766</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1962,13 +2106,13 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>100.5385274468751</v>
+        <v>78.94641358631799</v>
       </c>
       <c r="C92">
-        <v>-0.4641533123331321</v>
+        <v>-0.149705052227932</v>
       </c>
       <c r="D92">
-        <v>0.9966713701571901</v>
+        <v>0.6953031389645636</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1976,13 +2120,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>100.9376213475724</v>
+        <v>79.01080157291747</v>
       </c>
       <c r="C93">
-        <v>-0.4699653594306659</v>
+        <v>-0.150642741353167</v>
       </c>
       <c r="D93">
-        <v>0.1527582076606218</v>
+        <v>0.4130895247730297</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1990,13 +2134,13 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>101.5943459520473</v>
+        <v>79.09685901145066</v>
       </c>
       <c r="C94">
-        <v>-0.4795293099812712</v>
+        <v>-0.1518960050211262</v>
       </c>
       <c r="D94">
-        <v>0.3665338245643951</v>
+        <v>0.2905728522333529</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2004,13 +2148,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>104.6524401869776</v>
+        <v>79.47607728532844</v>
       </c>
       <c r="C95">
-        <v>-0.5240646629171493</v>
+        <v>-0.1574186012426473</v>
       </c>
       <c r="D95">
-        <v>0.2559735297086234</v>
+        <v>0.9807375484191767</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2018,13 +2162,13 @@
         <v>98</v>
       </c>
       <c r="B96">
-        <v>109.4431228689974</v>
+        <v>79.59455167851539</v>
       </c>
       <c r="C96">
-        <v>-0.5938318864417103</v>
+        <v>-0.1591439564832338</v>
       </c>
       <c r="D96">
-        <v>0.1303520306870361</v>
+        <v>0.7651051190576664</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2032,13 +2176,13 @@
         <v>99</v>
       </c>
       <c r="B97">
-        <v>110.4908754093416</v>
+        <v>79.68868705857257</v>
       </c>
       <c r="C97">
-        <v>-0.6090904185826447</v>
+        <v>-0.1605148600762996</v>
       </c>
       <c r="D97">
-        <v>0.3114538632409835</v>
+        <v>0.3292717806970011</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2046,13 +2190,13 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>115.336425259874</v>
+        <v>80.24069309148</v>
       </c>
       <c r="C98">
-        <v>-0.6796566785418547</v>
+        <v>-0.1685537828856309</v>
       </c>
       <c r="D98">
-        <v>0.2698674185458157</v>
+        <v>0.148255465826315</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2060,13 +2204,685 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>118.3456471463514</v>
+        <v>80.43133005948987</v>
       </c>
       <c r="C99">
-        <v>-0.7234802982478366</v>
+        <v>-0.1713300494100465</v>
       </c>
       <c r="D99">
-        <v>0.6190769426398308</v>
+        <v>0.9975936722069609</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100">
+        <v>80.66968390569619</v>
+      </c>
+      <c r="C100">
+        <v>-0.1748012219276143</v>
+      </c>
+      <c r="D100">
+        <v>0.1416730786053116</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101">
+        <v>80.82838768475192</v>
+      </c>
+      <c r="C101">
+        <v>-0.1771124420109502</v>
+      </c>
+      <c r="D101">
+        <v>0.08337801878428561</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102">
+        <v>80.840747235211</v>
+      </c>
+      <c r="C102">
+        <v>-0.1772924354642378</v>
+      </c>
+      <c r="D102">
+        <v>0.3330612730474438</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103">
+        <v>80.96309841454418</v>
+      </c>
+      <c r="C103">
+        <v>-0.1790742487554977</v>
+      </c>
+      <c r="D103">
+        <v>0.1713766902312611</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104">
+        <v>81.24885345351547</v>
+      </c>
+      <c r="C104">
+        <v>-0.1832357299055651</v>
+      </c>
+      <c r="D104">
+        <v>0.6589382005900397</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105">
+        <v>81.31775910080978</v>
+      </c>
+      <c r="C105">
+        <v>-0.1842392102059678</v>
+      </c>
+      <c r="D105">
+        <v>0.203804413452341</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106">
+        <v>81.38507834503407</v>
+      </c>
+      <c r="C106">
+        <v>-0.1852195875490399</v>
+      </c>
+      <c r="D106">
+        <v>0.1993899118485667</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107">
+        <v>81.48315140098211</v>
+      </c>
+      <c r="C107">
+        <v>-0.1866478359366328</v>
+      </c>
+      <c r="D107">
+        <v>0.2446118030781931</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108">
+        <v>81.58915486120378</v>
+      </c>
+      <c r="C108">
+        <v>-0.1881915756485986</v>
+      </c>
+      <c r="D108">
+        <v>0.1505632295690919</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109">
+        <v>81.83315479892742</v>
+      </c>
+      <c r="C109">
+        <v>-0.1917449727999141</v>
+      </c>
+      <c r="D109">
+        <v>0.4296908033270678</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110">
+        <v>82.10972628458939</v>
+      </c>
+      <c r="C110">
+        <v>-0.1957727128823699</v>
+      </c>
+      <c r="D110">
+        <v>0.2775241700914855</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111">
+        <v>83.00024606930707</v>
+      </c>
+      <c r="C111">
+        <v>-0.2087414476112679</v>
+      </c>
+      <c r="D111">
+        <v>0.3069100089954692</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112">
+        <v>83.06346401768675</v>
+      </c>
+      <c r="C112">
+        <v>-0.2096620973449528</v>
+      </c>
+      <c r="D112">
+        <v>0.3097120793620877</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113">
+        <v>83.1037872509887</v>
+      </c>
+      <c r="C113">
+        <v>-0.2102493288978937</v>
+      </c>
+      <c r="D113">
+        <v>0.3710261286206842</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114">
+        <v>83.27253817449051</v>
+      </c>
+      <c r="C114">
+        <v>-0.2127068666187937</v>
+      </c>
+      <c r="D114">
+        <v>0.1371629033638607</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115">
+        <v>83.77609615225529</v>
+      </c>
+      <c r="C115">
+        <v>-0.2200402352270188</v>
+      </c>
+      <c r="D115">
+        <v>0.2736171918729086</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116">
+        <v>83.95523339668414</v>
+      </c>
+      <c r="C116">
+        <v>-0.222649030048798</v>
+      </c>
+      <c r="D116">
+        <v>0.4201386962258283</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117">
+        <v>84.22423535887931</v>
+      </c>
+      <c r="C117">
+        <v>-0.2265665343526113</v>
+      </c>
+      <c r="D117">
+        <v>0.4841432660102745</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118">
+        <v>84.38213490639438</v>
+      </c>
+      <c r="C118">
+        <v>-0.2288660423261319</v>
+      </c>
+      <c r="D118">
+        <v>0.2588600371104243</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119">
+        <v>84.41413627864227</v>
+      </c>
+      <c r="C119">
+        <v>-0.2293320817278002</v>
+      </c>
+      <c r="D119">
+        <v>0.5951594464996305</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>122</v>
+      </c>
+      <c r="B120">
+        <v>84.4609864682877</v>
+      </c>
+      <c r="C120">
+        <v>-0.2300143660430247</v>
+      </c>
+      <c r="D120">
+        <v>0.3304020499520942</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121">
+        <v>84.48801735346662</v>
+      </c>
+      <c r="C121">
+        <v>-0.2304080197106788</v>
+      </c>
+      <c r="D121">
+        <v>0.428551982564824</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122">
+        <v>84.50126596207663</v>
+      </c>
+      <c r="C122">
+        <v>-0.2306009606127666</v>
+      </c>
+      <c r="D122">
+        <v>0.34944441961738</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123">
+        <v>84.51450446143988</v>
+      </c>
+      <c r="C123">
+        <v>-0.2307937542928138</v>
+      </c>
+      <c r="D123">
+        <v>0.2838303699742598</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124">
+        <v>84.63138068523709</v>
+      </c>
+      <c r="C124">
+        <v>-0.2324958352218993</v>
+      </c>
+      <c r="D124">
+        <v>0.9847962266856953</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125">
+        <v>85.05754229106175</v>
+      </c>
+      <c r="C125">
+        <v>-0.2387020721999285</v>
+      </c>
+      <c r="D125">
+        <v>0.7514098144694404</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126">
+        <v>85.44907748210626</v>
+      </c>
+      <c r="C126">
+        <v>-0.2444040410015476</v>
+      </c>
+      <c r="D126">
+        <v>0.5670531569500559</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127">
+        <v>85.59916612822541</v>
+      </c>
+      <c r="C127">
+        <v>-0.2465897979838652</v>
+      </c>
+      <c r="D127">
+        <v>0.4401499823417948</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128">
+        <v>85.82747016927884</v>
+      </c>
+      <c r="C128">
+        <v>-0.2499146141157114</v>
+      </c>
+      <c r="D128">
+        <v>0.2554664197001267</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129">
+        <v>87.01468823926163</v>
+      </c>
+      <c r="C129">
+        <v>-0.2672041976591499</v>
+      </c>
+      <c r="D129">
+        <v>0.2244901419159497</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130">
+        <v>87.35928801817067</v>
+      </c>
+      <c r="C130">
+        <v>-0.2722226410413204</v>
+      </c>
+      <c r="D130">
+        <v>0.2555623485599013</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131">
+        <v>87.99837015020408</v>
+      </c>
+      <c r="C131">
+        <v>-0.2815296623816128</v>
+      </c>
+      <c r="D131">
+        <v>0.3322824680896144</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132">
+        <v>88.85219042669786</v>
+      </c>
+      <c r="C132">
+        <v>-0.2939639382528816</v>
+      </c>
+      <c r="D132">
+        <v>0.6742132029585036</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133">
+        <v>89.33907163595471</v>
+      </c>
+      <c r="C133">
+        <v>-0.3010544413003113</v>
+      </c>
+      <c r="D133">
+        <v>0.230650967160605</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134">
+        <v>89.41611853142362</v>
+      </c>
+      <c r="C134">
+        <v>-0.3021764834673344</v>
+      </c>
+      <c r="D134">
+        <v>0.282467135484367</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135">
+        <v>90.37850164849409</v>
+      </c>
+      <c r="C135">
+        <v>-0.3161917715800111</v>
+      </c>
+      <c r="D135">
+        <v>0.3460522953470555</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136">
+        <v>91.31252167992336</v>
+      </c>
+      <c r="C136">
+        <v>-0.3297940050474277</v>
+      </c>
+      <c r="D136">
+        <v>0.2501839461760147</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137">
+        <v>91.88172229083797</v>
+      </c>
+      <c r="C137">
+        <v>-0.3380833343325917</v>
+      </c>
+      <c r="D137">
+        <v>0.8206075878329422</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138">
+        <v>92.2241358787024</v>
+      </c>
+      <c r="C138">
+        <v>-0.343069939981103</v>
+      </c>
+      <c r="D138">
+        <v>0.4864067039192819</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139">
+        <v>92.88911336226195</v>
+      </c>
+      <c r="C139">
+        <v>-0.3527540780911935</v>
+      </c>
+      <c r="D139">
+        <v>0.1651511108319181</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140">
+        <v>93.87533346030274</v>
+      </c>
+      <c r="C140">
+        <v>-0.3671165067034379</v>
+      </c>
+      <c r="D140">
+        <v>0.9754084285618934</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141">
+        <v>94.01406264248074</v>
+      </c>
+      <c r="C141">
+        <v>-0.3691368345992341</v>
+      </c>
+      <c r="D141">
+        <v>0.9690139452219071</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142">
+        <v>98.06783892599968</v>
+      </c>
+      <c r="C142">
+        <v>-0.4281724115436847</v>
+      </c>
+      <c r="D142">
+        <v>0.2453635683171555</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>145</v>
+      </c>
+      <c r="B143">
+        <v>99.57224708327142</v>
+      </c>
+      <c r="C143">
+        <v>-0.450081268202982</v>
+      </c>
+      <c r="D143">
+        <v>0.8255009348831179</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144">
+        <v>100.0580636996499</v>
+      </c>
+      <c r="C144">
+        <v>-0.4571562674706295</v>
+      </c>
+      <c r="D144">
+        <v>0.7403050318683571</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145">
+        <v>100.0793998306919</v>
+      </c>
+      <c r="C145">
+        <v>-0.4574669878256103</v>
+      </c>
+      <c r="D145">
+        <v>0.16948127664422</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>148</v>
+      </c>
+      <c r="B146">
+        <v>108.5425557329339</v>
+      </c>
+      <c r="C146">
+        <v>-0.580716831062144</v>
+      </c>
+      <c r="D146">
+        <v>0.1835347267707517</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147">
+        <v>115.5165466485376</v>
+      </c>
+      <c r="C147">
+        <v>-0.6822798055612274</v>
+      </c>
+      <c r="D147">
+        <v>0.3723213575836608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup: Wed Jan  1 23:06:49 IST 2025
</commit_message>
<xml_diff>
--- a/linear_regression_with_significance.xlsx
+++ b/linear_regression_with_significance.xlsx
@@ -31,436 +31,436 @@
     <t>Frontal Pole Volume Avg</t>
   </si>
   <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
     <t>Frontal Pole Volume Change</t>
   </si>
   <si>
-    <t>Temporal Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+    <t xml:space="preserve">age at baseline </t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Change</t>
   </si>
   <si>
     <t>Superior Parietal Lobule Volume Change</t>
   </si>
   <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
     <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
   </si>
   <si>
-    <t>Lateral Occipital Cortex, superior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Avg</t>
+    <t>Supracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
   </si>
   <si>
     <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
   </si>
   <si>
-    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Avg</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Avg</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age at baseline </t>
+    <t>Frontal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Change</t>
   </si>
   <si>
     <t>Inferior Temporal Gyrus, posterior division Change</t>
   </si>
   <si>
-    <t>Middle Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Change</t>
+    <t>Cingulate Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Change</t>
   </si>
   <si>
     <t>Precuneous Cortex Change</t>
   </si>
   <si>
-    <t>Insular Cortex Change</t>
+    <t>Frontal Pole Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
   </si>
   <si>
     <t>Paracingulate Gyrus Change</t>
   </si>
   <si>
-    <t>Middle Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
+    <t>Superior Parietal Lobule Change</t>
   </si>
   <si>
     <t>Supramarginal Gyrus, posterior division Change</t>
   </si>
   <si>
-    <t>Cingulate Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Change</t>
+    <t>Middle Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Change</t>
   </si>
   <si>
     <t>Angular Gyrus Change</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Change</t>
   </si>
 </sst>
 </file>
@@ -843,13 +843,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>60.17164266905188</v>
+        <v>55.54202081773011</v>
       </c>
       <c r="C2">
-        <v>0.1237139417128367</v>
+        <v>0.1911356191592701</v>
       </c>
       <c r="D2">
-        <v>0.05415189245990559</v>
+        <v>0.05279187603332048</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -857,13 +857,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>65.60641941254023</v>
+        <v>60.41752672616147</v>
       </c>
       <c r="C3">
-        <v>0.04456670758436543</v>
+        <v>0.1201331059296874</v>
       </c>
       <c r="D3">
-        <v>0.3097875730287992</v>
+        <v>0.06112447544471123</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -871,13 +871,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>68.80617111857266</v>
+        <v>61.07141577331057</v>
       </c>
       <c r="C4">
-        <v>-0.002031618231640886</v>
+        <v>0.1106104499032442</v>
       </c>
       <c r="D4">
-        <v>0.2513486097835893</v>
+        <v>0.05287306437930851</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -885,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>68.98895941840277</v>
+        <v>63.4655907086429</v>
       </c>
       <c r="C5">
-        <v>-0.004693583763147213</v>
+        <v>0.07574382463141416</v>
       </c>
       <c r="D5">
-        <v>0.43233424650578</v>
+        <v>0.2239066625532428</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -899,13 +899,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>68.98895941840277</v>
+        <v>64.52744180229787</v>
       </c>
       <c r="C6">
-        <v>-0.004693583763147213</v>
+        <v>0.06027997375294358</v>
       </c>
       <c r="D6">
-        <v>0.4323342465057802</v>
+        <v>0.2762699270416408</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -913,13 +913,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>68.98895941840277</v>
+        <v>64.8906118629907</v>
       </c>
       <c r="C7">
-        <v>-0.004693583763147213</v>
+        <v>0.05499108937392194</v>
       </c>
       <c r="D7">
-        <v>0.4323342465057808</v>
+        <v>0.2326623324699504</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -927,13 +927,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>68.9889594184028</v>
+        <v>64.94838171743879</v>
       </c>
       <c r="C8">
-        <v>-0.004693583763147657</v>
+        <v>0.05414978081399813</v>
       </c>
       <c r="D8">
-        <v>0.4323342465057549</v>
+        <v>0.2204292672352802</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -941,13 +941,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>68.9889594184028</v>
+        <v>65.62484253401277</v>
       </c>
       <c r="C9">
-        <v>-0.004693583763147657</v>
+        <v>0.04429840969884302</v>
       </c>
       <c r="D9">
-        <v>0.4323342465057608</v>
+        <v>0.06122981799759784</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -955,13 +955,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>68.98895941840691</v>
+        <v>66.6513888254446</v>
       </c>
       <c r="C10">
-        <v>-0.004693583763207387</v>
+        <v>0.0293487064255642</v>
       </c>
       <c r="D10">
-        <v>0.4323342465055366</v>
+        <v>0.2396312773643319</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -969,13 +969,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>69.18146333620285</v>
+        <v>67.22290084466719</v>
       </c>
       <c r="C11">
-        <v>-0.00749703887674058</v>
+        <v>0.0210257158543613</v>
       </c>
       <c r="D11">
-        <v>0.8572249109978035</v>
+        <v>0.3590941830306501</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -983,10 +983,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>69.24058769513314</v>
+        <v>67.4183338034219</v>
       </c>
       <c r="C12">
-        <v>-0.008358073230094298</v>
+        <v>0.0181796048045354</v>
+      </c>
+      <c r="D12">
+        <v>0.3843822982127002</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -994,10 +997,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>69.24058769513314</v>
+        <v>67.51205211794567</v>
       </c>
       <c r="C13">
-        <v>-0.008358073230094298</v>
+        <v>0.01681477498137363</v>
+      </c>
+      <c r="D13">
+        <v>0.4056856226221157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1005,10 +1011,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>69.24058769513314</v>
+        <v>67.59410185777965</v>
       </c>
       <c r="C14">
-        <v>-0.008358073230094298</v>
+        <v>0.01561987585757796</v>
+      </c>
+      <c r="D14">
+        <v>0.4447907238901564</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1016,10 +1025,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>69.24058769513314</v>
+        <v>67.80414079965385</v>
       </c>
       <c r="C15">
-        <v>-0.008358073230094298</v>
+        <v>0.01256105631572058</v>
+      </c>
+      <c r="D15">
+        <v>0.550651527199203</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1027,714 +1039,909 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>69.24058769513314</v>
+        <v>68.02061569407579</v>
       </c>
       <c r="C16">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>0.00940850930957593</v>
+      </c>
+      <c r="D16">
+        <v>0.4684520375045017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17">
-        <v>69.24058769513314</v>
+        <v>68.21686793519677</v>
       </c>
       <c r="C17">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>0.006550466963153756</v>
+      </c>
+      <c r="D17">
+        <v>0.5507431244906833</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18">
-        <v>69.24058769513314</v>
+        <v>68.25051687217841</v>
       </c>
       <c r="C18">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>0.00606043390031441</v>
+      </c>
+      <c r="D18">
+        <v>0.590012499156545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19">
-        <v>69.24058769513314</v>
+        <v>68.32098716091679</v>
       </c>
       <c r="C19">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>0.005034167559464398</v>
+      </c>
+      <c r="D19">
+        <v>0.4025143907045666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
-        <v>69.24058769513314</v>
+        <v>68.38071128778341</v>
       </c>
       <c r="C20">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>0.004164398721600904</v>
+      </c>
+      <c r="D20">
+        <v>0.5865971475663934</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
-        <v>69.24058769513314</v>
+        <v>68.47809290147293</v>
       </c>
       <c r="C21">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>0.002746219881462175</v>
+      </c>
+      <c r="D21">
+        <v>0.6100421788994763</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22">
-        <v>69.24058769513314</v>
+        <v>68.49987697929187</v>
       </c>
       <c r="C22">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>0.002428976029730023</v>
+      </c>
+      <c r="D22">
+        <v>0.5353861247105034</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23">
-        <v>69.24058769513314</v>
+        <v>68.54771342131046</v>
       </c>
       <c r="C23">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>0.001732328815866935</v>
+      </c>
+      <c r="D23">
+        <v>0.6017612687645815</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24">
-        <v>69.24058769513314</v>
+        <v>68.67177649513013</v>
       </c>
       <c r="C24">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>-7.441497762328275E-05</v>
+      </c>
+      <c r="D24">
+        <v>0.3221087969052605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25">
-        <v>69.24058769513314</v>
+        <v>68.83043204145818</v>
       </c>
       <c r="C25">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>-0.002384932642594872</v>
+      </c>
+      <c r="D25">
+        <v>0.6343160103450627</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26">
-        <v>69.24058769513314</v>
+        <v>69.00943452746645</v>
       </c>
       <c r="C26">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>-0.004991764963103718</v>
+      </c>
+      <c r="D26">
+        <v>0.8076779085040482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27">
-        <v>69.24058769513314</v>
+        <v>69.04182505902726</v>
       </c>
       <c r="C27">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>-0.005463471733406777</v>
+      </c>
+      <c r="D27">
+        <v>0.6210298847256009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28">
-        <v>69.24058769513314</v>
+        <v>69.05964728042945</v>
       </c>
       <c r="C28">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>-0.005723018647030731</v>
+      </c>
+      <c r="D28">
+        <v>0.7630940607759764</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29">
-        <v>69.24058769513314</v>
+        <v>69.08496481839377</v>
       </c>
       <c r="C29">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>-0.006091720656220101</v>
+      </c>
+      <c r="D29">
+        <v>0.5476313920376215</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30">
-        <v>69.24058769513314</v>
+        <v>69.18168494670948</v>
       </c>
       <c r="C30">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>-0.007500266214215845</v>
+      </c>
+      <c r="D30">
+        <v>0.8100519433945763</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>33</v>
       </c>
       <c r="B31">
-        <v>69.24058769513314</v>
+        <v>69.18857660246675</v>
       </c>
       <c r="C31">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>-0.007600630133011155</v>
+      </c>
+      <c r="D31">
+        <v>0.7352002814750809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>34</v>
       </c>
       <c r="B32">
-        <v>69.24058769513314</v>
+        <v>69.21633982466746</v>
       </c>
       <c r="C32">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>-0.008004948902924136</v>
+      </c>
+      <c r="D32">
+        <v>0.03562289372370342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33">
-        <v>69.24058769513314</v>
+        <v>69.29651490988087</v>
       </c>
       <c r="C33">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>-0.009172547231274919</v>
+      </c>
+      <c r="D33">
+        <v>0.4087193821993432</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>36</v>
       </c>
       <c r="B34">
-        <v>69.24058769513314</v>
+        <v>69.30006141437428</v>
       </c>
       <c r="C34">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>-0.009224195354965437</v>
+      </c>
+      <c r="D34">
+        <v>0.4388105046984263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>37</v>
       </c>
       <c r="B35">
-        <v>69.24058769513314</v>
+        <v>69.34298140836728</v>
       </c>
       <c r="C35">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>-0.009849243811173913</v>
+      </c>
+      <c r="D35">
+        <v>0.8751914167575987</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>38</v>
       </c>
       <c r="B36">
-        <v>69.24058769513314</v>
+        <v>69.39469920510095</v>
       </c>
       <c r="C36">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>-0.01060241560826625</v>
+      </c>
+      <c r="D36">
+        <v>0.998948466201195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37">
-        <v>69.24058769513314</v>
+        <v>69.44168618555629</v>
       </c>
       <c r="C37">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>-0.01128669202266441</v>
+      </c>
+      <c r="D37">
+        <v>0.9461287414802102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>40</v>
       </c>
       <c r="B38">
-        <v>69.24058769513314</v>
+        <v>69.53708624176514</v>
       </c>
       <c r="C38">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>-0.01267601322958933</v>
+      </c>
+      <c r="D38">
+        <v>0.1597869090806618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="B39">
-        <v>69.24058769513314</v>
+        <v>69.61708791345816</v>
       </c>
       <c r="C39">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>-0.01384108611832269</v>
+      </c>
+      <c r="D39">
+        <v>0.9566496111225951</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>42</v>
       </c>
       <c r="B40">
-        <v>69.24058769513314</v>
+        <v>69.73305765982361</v>
       </c>
       <c r="C40">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>-0.01552996591976141</v>
+      </c>
+      <c r="D40">
+        <v>0.498124836369502</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>43</v>
       </c>
       <c r="B41">
-        <v>69.24058769513314</v>
+        <v>69.82921431641626</v>
       </c>
       <c r="C41">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>-0.01693030557887742</v>
+      </c>
+      <c r="D41">
+        <v>0.9101854880917394</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>44</v>
       </c>
       <c r="B42">
-        <v>69.24058769513314</v>
+        <v>69.83195989077272</v>
       </c>
       <c r="C42">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>-0.01697028967144742</v>
+      </c>
+      <c r="D42">
+        <v>0.9305282233166774</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43">
-        <v>69.24058769513314</v>
+        <v>69.85046687938711</v>
       </c>
       <c r="C43">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>-0.01723980892311339</v>
+      </c>
+      <c r="D43">
+        <v>0.5254703628853179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44">
-        <v>69.24058769513314</v>
+        <v>69.85688532454452</v>
       </c>
       <c r="C44">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>-0.01733328142540547</v>
+      </c>
+      <c r="D44">
+        <v>0.8364136660964817</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>47</v>
       </c>
       <c r="B45">
-        <v>69.24058769513314</v>
+        <v>69.86544975791065</v>
       </c>
       <c r="C45">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>-0.01745800618316484</v>
+      </c>
+      <c r="D45">
+        <v>0.490852013882599</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46">
-        <v>69.24058769513314</v>
+        <v>69.88207352119618</v>
       </c>
       <c r="C46">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>-0.01770009982324527</v>
+      </c>
+      <c r="D46">
+        <v>0.5270967494510257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>49</v>
       </c>
       <c r="B47">
-        <v>69.24058769513314</v>
+        <v>70.02863807811531</v>
       </c>
       <c r="C47">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>-0.01983453511818412</v>
+      </c>
+      <c r="D47">
+        <v>0.8895010247528776</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>50</v>
       </c>
       <c r="B48">
-        <v>69.24058769513314</v>
+        <v>70.08901580320889</v>
       </c>
       <c r="C48">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>-0.02071382237682862</v>
+      </c>
+      <c r="D48">
+        <v>0.8406279839112907</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>51</v>
       </c>
       <c r="B49">
-        <v>69.24058769513314</v>
+        <v>70.17031557141169</v>
       </c>
       <c r="C49">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>-0.02189779958366556</v>
+      </c>
+      <c r="D49">
+        <v>0.5724729481208475</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>52</v>
       </c>
       <c r="B50">
-        <v>69.24058769513314</v>
+        <v>70.22515261390623</v>
       </c>
       <c r="C50">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>-0.02269639728989659</v>
+      </c>
+      <c r="D50">
+        <v>0.9724700730256017</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>53</v>
       </c>
       <c r="B51">
-        <v>69.24058769513314</v>
+        <v>70.24960434154804</v>
       </c>
       <c r="C51">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>-0.02305249041089374</v>
+      </c>
+      <c r="D51">
+        <v>0.6731288165574267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>54</v>
       </c>
       <c r="B52">
-        <v>69.24058769513314</v>
+        <v>70.31389504475381</v>
       </c>
       <c r="C52">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>-0.02398876278767692</v>
+      </c>
+      <c r="D52">
+        <v>0.7130037887185959</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>55</v>
       </c>
       <c r="B53">
-        <v>69.24058769513314</v>
+        <v>70.41351154870434</v>
       </c>
       <c r="C53">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>-0.0254394885733642</v>
+      </c>
+      <c r="D53">
+        <v>0.752997486680917</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>56</v>
       </c>
       <c r="B54">
-        <v>69.24058769513314</v>
+        <v>70.62662373793543</v>
       </c>
       <c r="C54">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>-0.02854306414469088</v>
+      </c>
+      <c r="D54">
+        <v>0.5959985032632197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>57</v>
       </c>
       <c r="B55">
-        <v>69.24058769513314</v>
+        <v>70.72061079274492</v>
       </c>
       <c r="C55">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>-0.02991180766133383</v>
+      </c>
+      <c r="D55">
+        <v>0.03800878798105314</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>58</v>
       </c>
       <c r="B56">
-        <v>69.24058769513314</v>
+        <v>70.77893538931397</v>
       </c>
       <c r="C56">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>-0.03076119499000929</v>
+      </c>
+      <c r="D56">
+        <v>0.6992242603346432</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>59</v>
       </c>
       <c r="B57">
-        <v>69.24058769513314</v>
+        <v>70.98905848622871</v>
       </c>
       <c r="C57">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>-0.03382124009070941</v>
+      </c>
+      <c r="D57">
+        <v>0.6288256261527839</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>60</v>
       </c>
       <c r="B58">
-        <v>69.24058769513314</v>
+        <v>71.18149853399399</v>
       </c>
       <c r="C58">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>-0.03662376505816489</v>
+      </c>
+      <c r="D58">
+        <v>0.771664349340643</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59">
-        <v>69.24058769513314</v>
+        <v>71.20807043654648</v>
       </c>
       <c r="C59">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>-0.03701073451281278</v>
+      </c>
+      <c r="D59">
+        <v>0.6542874573175916</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>62</v>
       </c>
       <c r="B60">
-        <v>69.24058769513314</v>
+        <v>71.21537666730381</v>
       </c>
       <c r="C60">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>-0.03711713593160915</v>
+      </c>
+      <c r="D60">
+        <v>0.07780434642915535</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>63</v>
       </c>
       <c r="B61">
-        <v>69.24058769513314</v>
+        <v>71.22643447325102</v>
       </c>
       <c r="C61">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>-0.03727817194054883</v>
+      </c>
+      <c r="D61">
+        <v>0.1145759339875331</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>64</v>
       </c>
       <c r="B62">
-        <v>69.24058769513314</v>
+        <v>71.23482563851836</v>
       </c>
       <c r="C62">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>-0.03740037337648094</v>
+      </c>
+      <c r="D62">
+        <v>0.1163006391407411</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>65</v>
       </c>
       <c r="B63">
-        <v>69.24058769513314</v>
+        <v>71.62458447463652</v>
       </c>
       <c r="C63">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>-0.04307647293159977</v>
+      </c>
+      <c r="D63">
+        <v>0.4182516193871859</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>66</v>
       </c>
       <c r="B64">
-        <v>69.24058769513314</v>
+        <v>71.76354420803904</v>
       </c>
       <c r="C64">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>-0.04510015836950054</v>
+      </c>
+      <c r="D64">
+        <v>0.2590674548641074</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>67</v>
       </c>
       <c r="B65">
-        <v>69.24058769513314</v>
+        <v>72.03860874525633</v>
       </c>
       <c r="C65">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>-0.04910595260082018</v>
+      </c>
+      <c r="D65">
+        <v>0.7741005029983061</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>68</v>
       </c>
       <c r="B66">
-        <v>69.24058769513314</v>
+        <v>72.05383022115026</v>
       </c>
       <c r="C66">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>-0.04932762457985818</v>
+      </c>
+      <c r="D66">
+        <v>0.6159789939789663</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>69</v>
       </c>
       <c r="B67">
-        <v>69.24058769513314</v>
+        <v>72.05620902818163</v>
       </c>
       <c r="C67">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>-0.04936226740070349</v>
+      </c>
+      <c r="D67">
+        <v>0.545905277550076</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>70</v>
       </c>
       <c r="B68">
-        <v>69.24058769513314</v>
+        <v>72.19097971272089</v>
       </c>
       <c r="C68">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>-0.05132494727263448</v>
+      </c>
+      <c r="D68">
+        <v>0.3948316531874997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>71</v>
       </c>
       <c r="B69">
-        <v>69.24058769513314</v>
+        <v>72.19565574624463</v>
       </c>
       <c r="C69">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>-0.05139304484822271</v>
+      </c>
+      <c r="D69">
+        <v>0.05224086509107263</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>72</v>
       </c>
       <c r="B70">
-        <v>69.24058769513314</v>
+        <v>72.27261253158173</v>
       </c>
       <c r="C70">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>-0.05251377473177254</v>
+      </c>
+      <c r="D70">
+        <v>0.3683686240214875</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71">
-        <v>69.24058769513314</v>
+        <v>72.4789438928867</v>
       </c>
       <c r="C71">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>-0.05551860038184531</v>
+      </c>
+      <c r="D71">
+        <v>0.4843417897480464</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>74</v>
       </c>
       <c r="B72">
-        <v>69.24058769513314</v>
+        <v>72.50071887577786</v>
       </c>
       <c r="C72">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>-0.05583571178317293</v>
+      </c>
+      <c r="D72">
+        <v>0.05714288744451292</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>75</v>
       </c>
       <c r="B73">
-        <v>69.24058769513314</v>
+        <v>72.65361118593795</v>
       </c>
       <c r="C73">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>-0.05806229882433911</v>
+      </c>
+      <c r="D73">
+        <v>0.6272481590341763</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74">
-        <v>69.24058769513314</v>
+        <v>72.68513033785204</v>
       </c>
       <c r="C74">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>-0.05852131559978702</v>
+      </c>
+      <c r="D74">
+        <v>0.6719229031495553</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>77</v>
       </c>
       <c r="B75">
-        <v>69.24058769513314</v>
+        <v>72.70463798734139</v>
       </c>
       <c r="C75">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>-0.05880540758264141</v>
+      </c>
+      <c r="D75">
+        <v>0.1963047371919701</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>78</v>
       </c>
       <c r="B76">
-        <v>69.24058769513314</v>
+        <v>72.76544338441994</v>
       </c>
       <c r="C76">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <v>-0.05969092307407697</v>
+      </c>
+      <c r="D76">
+        <v>0.821733778338277</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77">
-        <v>69.24058769513314</v>
+        <v>72.8750271996623</v>
       </c>
       <c r="C77">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>-0.06128680387857721</v>
+      </c>
+      <c r="D77">
+        <v>0.319199545339699</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>80</v>
       </c>
       <c r="B78">
-        <v>69.24058769513314</v>
+        <v>72.90094087057615</v>
       </c>
       <c r="C78">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>-0.061664187435575</v>
+      </c>
+      <c r="D78">
+        <v>0.00887383526854609</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79">
-        <v>69.24058769513314</v>
+        <v>73.10580274306524</v>
       </c>
       <c r="C79">
-        <v>-0.008358073230094298</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>-0.06464761276308617</v>
+      </c>
+      <c r="D79">
+        <v>0.5360903821672427</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>82</v>
       </c>
       <c r="B80">
-        <v>69.24058769513314</v>
+        <v>73.11216917677024</v>
       </c>
       <c r="C80">
-        <v>-0.008358073230094298</v>
+        <v>-0.0647403278170422</v>
+      </c>
+      <c r="D80">
+        <v>0.4228408208636953</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1742,10 +1949,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>69.24058769513314</v>
+        <v>73.12103271424225</v>
       </c>
       <c r="C81">
-        <v>-0.008358073230094298</v>
+        <v>-0.06486940845983846</v>
+      </c>
+      <c r="D81">
+        <v>0.1174649469213347</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1753,10 +1963,13 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>69.24058769513314</v>
+        <v>73.161147110032</v>
       </c>
       <c r="C82">
-        <v>-0.008358073230094298</v>
+        <v>-0.06545359868978662</v>
+      </c>
+      <c r="D82">
+        <v>0.1251405111592915</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1764,10 +1977,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>69.24058769513314</v>
+        <v>73.2931638878888</v>
       </c>
       <c r="C83">
-        <v>-0.008358073230094298</v>
+        <v>-0.0673761731245941</v>
+      </c>
+      <c r="D83">
+        <v>0.9702461192060646</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1775,10 +1991,13 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>69.24058769513314</v>
+        <v>73.29696890749015</v>
       </c>
       <c r="C84">
-        <v>-0.008358073230094298</v>
+        <v>-0.06743158603141008</v>
+      </c>
+      <c r="D84">
+        <v>0.101888757366417</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1786,10 +2005,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>69.24058769513314</v>
+        <v>73.60071087226467</v>
       </c>
       <c r="C85">
-        <v>-0.008358073230094298</v>
+        <v>-0.07185501270288364</v>
+      </c>
+      <c r="D85">
+        <v>0.4918852215887154</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1797,10 +2019,13 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>69.24058769513314</v>
+        <v>73.65913795511882</v>
       </c>
       <c r="C86">
-        <v>-0.008358073230094298</v>
+        <v>-0.07270589255027415</v>
+      </c>
+      <c r="D86">
+        <v>0.162323728445789</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1808,10 +2033,13 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>69.24058769513314</v>
+        <v>73.7104171550109</v>
       </c>
       <c r="C87">
-        <v>-0.008358073230094298</v>
+        <v>-0.07345267701472191</v>
+      </c>
+      <c r="D87">
+        <v>0.7751121850913547</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1819,10 +2047,13 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>69.24058769513314</v>
+        <v>73.71316207677627</v>
       </c>
       <c r="C88">
-        <v>-0.008358073230094298</v>
+        <v>-0.07349265160353791</v>
+      </c>
+      <c r="D88">
+        <v>0.1326884892573001</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1830,10 +2061,13 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>69.24058769513314</v>
+        <v>73.98451824771466</v>
       </c>
       <c r="C89">
-        <v>-0.008358073230094298</v>
+        <v>-0.07744444050069887</v>
+      </c>
+      <c r="D89">
+        <v>0.4296481439261044</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1841,10 +2075,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>69.24058769513314</v>
+        <v>74.0626337073423</v>
       </c>
       <c r="C90">
-        <v>-0.008358073230094298</v>
+        <v>-0.07858204428168403</v>
+      </c>
+      <c r="D90">
+        <v>0.497459911239897</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1852,10 +2089,13 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>69.24058769513314</v>
+        <v>74.13199491456501</v>
       </c>
       <c r="C91">
-        <v>-0.008358073230094298</v>
+        <v>-0.07959215894997596</v>
+      </c>
+      <c r="D91">
+        <v>0.5291293396105173</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1863,13 +2103,13 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>69.38739691840124</v>
+        <v>74.13259831064728</v>
       </c>
       <c r="C92">
-        <v>-0.01049607162720245</v>
+        <v>-0.07960094627156233</v>
       </c>
       <c r="D92">
-        <v>0.7289247120853499</v>
+        <v>0.13844047464105</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1877,13 +2117,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>69.38739691840277</v>
+        <v>74.30647085706134</v>
       </c>
       <c r="C93">
-        <v>-0.01049607162722488</v>
+        <v>-0.08213307073390297</v>
       </c>
       <c r="D93">
-        <v>0.7289247120827103</v>
+        <v>0.3874311337441763</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1891,13 +2131,13 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>69.62145321803213</v>
+        <v>74.61859849209365</v>
       </c>
       <c r="C94">
-        <v>-0.01390465851503109</v>
+        <v>-0.08667861881689776</v>
       </c>
       <c r="D94">
-        <v>0.4298204963732927</v>
+        <v>0.8976683566818522</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1905,13 +2145,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>69.75865612962461</v>
+        <v>74.89313439566257</v>
       </c>
       <c r="C95">
-        <v>-0.0159027591692904</v>
+        <v>-0.09067671449994053</v>
       </c>
       <c r="D95">
-        <v>0.4269632243972528</v>
+        <v>0.2950987867948573</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1919,13 +2159,13 @@
         <v>98</v>
       </c>
       <c r="B96">
-        <v>71.30581661677321</v>
+        <v>74.91723805327581</v>
       </c>
       <c r="C96">
-        <v>-0.03843422257436724</v>
+        <v>-0.09102773863993896</v>
       </c>
       <c r="D96">
-        <v>0.5840093026066006</v>
+        <v>0.9278424656488063</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1933,13 +2173,13 @@
         <v>99</v>
       </c>
       <c r="B97">
-        <v>71.30581661677323</v>
+        <v>75.16934553405025</v>
       </c>
       <c r="C97">
-        <v>-0.03843422257436746</v>
+        <v>-0.09469920680655708</v>
       </c>
       <c r="D97">
-        <v>0.5840093026066022</v>
+        <v>0.1111094374854422</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1947,13 +2187,13 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>78.04832652780568</v>
+        <v>75.26856224306069</v>
       </c>
       <c r="C98">
-        <v>-0.1366261144826071</v>
+        <v>-0.09614411033583536</v>
       </c>
       <c r="D98">
-        <v>0.1993894770059438</v>
+        <v>0.09226146958348402</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1961,13 +2201,13 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>82.21417778953837</v>
+        <v>75.29235353433367</v>
       </c>
       <c r="C99">
-        <v>-0.1972938513039568</v>
+        <v>-0.09649058545146127</v>
       </c>
       <c r="D99">
-        <v>0.5899030893483257</v>
+        <v>0.3409550655347707</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1975,13 +2215,13 @@
         <v>102</v>
       </c>
       <c r="B100">
-        <v>82.65100730504297</v>
+        <v>75.34077379563284</v>
       </c>
       <c r="C100">
-        <v>-0.2036554461899462</v>
+        <v>-0.09719573488785693</v>
       </c>
       <c r="D100">
-        <v>0.3256748822267328</v>
+        <v>0.2186456991050574</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1989,13 +2229,13 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>84.27448131459727</v>
+        <v>75.43389954537813</v>
       </c>
       <c r="C101">
-        <v>-0.2272982715718048</v>
+        <v>-0.098551935126866</v>
       </c>
       <c r="D101">
-        <v>0.7059468346527491</v>
+        <v>0.6436681146391308</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2003,13 +2243,13 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>85.33446338376862</v>
+        <v>75.48258320289968</v>
       </c>
       <c r="C102">
-        <v>-0.2427349036471158</v>
+        <v>-0.09926092043057788</v>
       </c>
       <c r="D102">
-        <v>0.715549529201195</v>
+        <v>0.1328872130873812</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2017,13 +2257,13 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>85.38790153785473</v>
+        <v>75.52293937361105</v>
       </c>
       <c r="C103">
-        <v>-0.2435131291920591</v>
+        <v>-0.09984863165452995</v>
       </c>
       <c r="D103">
-        <v>0.8850132658878109</v>
+        <v>0.1317736248989538</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2031,13 +2271,13 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>86.78254247050833</v>
+        <v>75.60148324056735</v>
       </c>
       <c r="C104">
-        <v>-0.2638234340365291</v>
+        <v>-0.1009924743771944</v>
       </c>
       <c r="D104">
-        <v>0.3031967817028152</v>
+        <v>0.2092419325749682</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2045,13 +2285,13 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>86.79387238006439</v>
+        <v>75.74154818583737</v>
       </c>
       <c r="C105">
-        <v>-0.2639884327193842</v>
+        <v>-0.1030322551335541</v>
       </c>
       <c r="D105">
-        <v>0.2616072840720172</v>
+        <v>0.4923645278197668</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2059,13 +2299,13 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>87.46274342441737</v>
+        <v>75.75911344173647</v>
       </c>
       <c r="C106">
-        <v>-0.2737292731711267</v>
+        <v>-0.1032880598311139</v>
       </c>
       <c r="D106">
-        <v>0.8502926855825396</v>
+        <v>0.1285763626914587</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2073,13 +2313,13 @@
         <v>109</v>
       </c>
       <c r="B107">
-        <v>87.7263036559257</v>
+        <v>75.96721543141253</v>
       </c>
       <c r="C107">
-        <v>-0.2775675289697919</v>
+        <v>-0.1063186713312505</v>
       </c>
       <c r="D107">
-        <v>0.2636903751539774</v>
+        <v>0.369190355059335</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2087,13 +2327,13 @@
         <v>110</v>
       </c>
       <c r="B108">
-        <v>87.7897085454547</v>
+        <v>76.22290216397577</v>
       </c>
       <c r="C108">
-        <v>-0.2784909011473986</v>
+        <v>-0.110042264523919</v>
       </c>
       <c r="D108">
-        <v>0.3749284220266343</v>
+        <v>0.149798050528452</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2101,13 +2341,13 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>87.83088710217265</v>
+        <v>76.49084418670549</v>
       </c>
       <c r="C109">
-        <v>-0.279090588866592</v>
+        <v>-0.1139443328160994</v>
       </c>
       <c r="D109">
-        <v>0.1804819273190955</v>
+        <v>0.04203691712059767</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2115,13 +2355,13 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>88.69546248816408</v>
+        <v>76.57821785601229</v>
       </c>
       <c r="C110">
-        <v>-0.2916814925460789</v>
+        <v>-0.1152167648933828</v>
       </c>
       <c r="D110">
-        <v>0.3986881634280947</v>
+        <v>0.551297681181437</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2129,13 +2369,13 @@
         <v>113</v>
       </c>
       <c r="B111">
-        <v>88.72793630257006</v>
+        <v>76.64224804114292</v>
       </c>
       <c r="C111">
-        <v>-0.2921544121733504</v>
+        <v>-0.1161492433176154</v>
       </c>
       <c r="D111">
-        <v>0.1597613874796744</v>
+        <v>0.009220522230884928</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2143,13 +2383,13 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>88.87695769873923</v>
+        <v>76.93326986368164</v>
       </c>
       <c r="C112">
-        <v>-0.2943246266806685</v>
+        <v>-0.1203874251992472</v>
       </c>
       <c r="D112">
-        <v>0.4615810791321999</v>
+        <v>0.153421811511493</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2157,13 +2397,13 @@
         <v>115</v>
       </c>
       <c r="B113">
-        <v>89.45829920099047</v>
+        <v>77.35496289372983</v>
       </c>
       <c r="C113">
-        <v>-0.302790765062968</v>
+        <v>-0.126528585831017</v>
       </c>
       <c r="D113">
-        <v>0.5522169465136547</v>
+        <v>0.157033176695222</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2171,13 +2411,13 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>90.73136026757862</v>
+        <v>77.40178075804917</v>
       </c>
       <c r="C114">
-        <v>-0.3213304893336693</v>
+        <v>-0.1272103993890656</v>
       </c>
       <c r="D114">
-        <v>0.351773084763663</v>
+        <v>0.9541721462265929</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2185,13 +2425,13 @@
         <v>117</v>
       </c>
       <c r="B115">
-        <v>91.08121286798054</v>
+        <v>77.51011673093114</v>
       </c>
       <c r="C115">
-        <v>-0.3264254301162215</v>
+        <v>-0.128788107732007</v>
       </c>
       <c r="D115">
-        <v>0.2010778932443412</v>
+        <v>0.2200283506934367</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2199,13 +2439,13 @@
         <v>118</v>
       </c>
       <c r="B116">
-        <v>91.32651361153233</v>
+        <v>77.61976330583501</v>
       </c>
       <c r="C116">
-        <v>-0.3299977710417332</v>
+        <v>-0.1303849025121604</v>
       </c>
       <c r="D116">
-        <v>0.1790952995532874</v>
+        <v>0.005412367384066267</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2213,13 +2453,13 @@
         <v>119</v>
       </c>
       <c r="B117">
-        <v>91.44860188623153</v>
+        <v>77.67216964458771</v>
       </c>
       <c r="C117">
-        <v>-0.3317757556247312</v>
+        <v>-0.1311481016202094</v>
       </c>
       <c r="D117">
-        <v>0.2223620116132827</v>
+        <v>0.8794862275341265</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2227,13 +2467,13 @@
         <v>120</v>
       </c>
       <c r="B118">
-        <v>92.04873290887622</v>
+        <v>78.04832652780568</v>
       </c>
       <c r="C118">
-        <v>-0.3405155277991683</v>
+        <v>-0.1366261144826071</v>
       </c>
       <c r="D118">
-        <v>0.3683110068255224</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2241,13 +2481,13 @@
         <v>121</v>
       </c>
       <c r="B119">
-        <v>92.42501234744608</v>
+        <v>78.21566079056869</v>
       </c>
       <c r="C119">
-        <v>-0.345995325448244</v>
+        <v>-0.1390630212218742</v>
       </c>
       <c r="D119">
-        <v>0.1718873587692883</v>
+        <v>0.2128049735853601</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2255,13 +2495,13 @@
         <v>122</v>
       </c>
       <c r="B120">
-        <v>92.85696191328871</v>
+        <v>78.29536958931622</v>
       </c>
       <c r="C120">
-        <v>-0.3522858531061464</v>
+        <v>-0.1402238289706246</v>
       </c>
       <c r="D120">
-        <v>0.2333407351586075</v>
+        <v>0.1459243744122649</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2269,13 +2509,13 @@
         <v>123</v>
       </c>
       <c r="B121">
-        <v>92.88593043791766</v>
+        <v>78.3716102651304</v>
       </c>
       <c r="C121">
-        <v>-0.3527077248240436</v>
+        <v>-0.1413341300747144</v>
       </c>
       <c r="D121">
-        <v>0.3306865701701599</v>
+        <v>0.092990422424097</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2283,13 +2523,13 @@
         <v>124</v>
       </c>
       <c r="B122">
-        <v>93.70120849941689</v>
+        <v>78.57220955481699</v>
       </c>
       <c r="C122">
-        <v>-0.3645807063021878</v>
+        <v>-0.1442554789536457</v>
       </c>
       <c r="D122">
-        <v>0.3100287825223316</v>
+        <v>0.3349481713517459</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2297,13 +2537,13 @@
         <v>125</v>
       </c>
       <c r="B123">
-        <v>94.32031813234904</v>
+        <v>78.78344687676518</v>
       </c>
       <c r="C123">
-        <v>-0.3735968660050832</v>
+        <v>-0.1473317506325027</v>
       </c>
       <c r="D123">
-        <v>0.2264767204763297</v>
+        <v>0.453334142204731</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2311,13 +2551,13 @@
         <v>126</v>
       </c>
       <c r="B124">
-        <v>94.52740412507033</v>
+        <v>78.84672576799851</v>
       </c>
       <c r="C124">
-        <v>-0.376612681433063</v>
+        <v>-0.1482532878834733</v>
       </c>
       <c r="D124">
-        <v>0.3209581326028851</v>
+        <v>0.1034381434860657</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2325,13 +2565,13 @@
         <v>127</v>
       </c>
       <c r="B125">
-        <v>95.38033792229314</v>
+        <v>79.11268053108718</v>
       </c>
       <c r="C125">
-        <v>-0.389034047412036</v>
+        <v>-0.1521264155012696</v>
       </c>
       <c r="D125">
-        <v>0.1709924939359675</v>
+        <v>0.02270697528117758</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2339,13 +2579,13 @@
         <v>128</v>
       </c>
       <c r="B126">
-        <v>96.11693949854687</v>
+        <v>79.35480458316975</v>
       </c>
       <c r="C126">
-        <v>-0.399761254833207</v>
+        <v>-0.1556524939296566</v>
       </c>
       <c r="D126">
-        <v>0.3840109273876789</v>
+        <v>0.06867740949709193</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2353,13 +2593,13 @@
         <v>129</v>
       </c>
       <c r="B127">
-        <v>97.17490792607663</v>
+        <v>79.82782480083107</v>
       </c>
       <c r="C127">
-        <v>-0.4151685620302423</v>
+        <v>-0.1625411378761805</v>
       </c>
       <c r="D127">
-        <v>0.1708037752382144</v>
+        <v>0.02750431193371585</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2367,13 +2607,13 @@
         <v>130</v>
       </c>
       <c r="B128">
-        <v>97.39111561947097</v>
+        <v>80.51115142493498</v>
       </c>
       <c r="C128">
-        <v>-0.418317217759286</v>
+        <v>-0.1724924964796355</v>
       </c>
       <c r="D128">
-        <v>0.4037486392822102</v>
+        <v>0.04173361010978927</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2381,13 +2621,13 @@
         <v>131</v>
       </c>
       <c r="B129">
-        <v>97.39806895417742</v>
+        <v>80.58956048240258</v>
       </c>
       <c r="C129">
-        <v>-0.4184184799152051</v>
+        <v>-0.1736343759573191</v>
       </c>
       <c r="D129">
-        <v>0.2474686684572161</v>
+        <v>0.1419051958502771</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2395,13 +2635,13 @@
         <v>132</v>
       </c>
       <c r="B130">
-        <v>97.53339963867224</v>
+        <v>80.71984632715981</v>
       </c>
       <c r="C130">
-        <v>-0.4203893151262947</v>
+        <v>-0.175531742628541</v>
       </c>
       <c r="D130">
-        <v>0.2519081946566925</v>
+        <v>0.05900138443219891</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2409,13 +2649,13 @@
         <v>133</v>
       </c>
       <c r="B131">
-        <v>97.81345355445586</v>
+        <v>80.81466310338456</v>
       </c>
       <c r="C131">
-        <v>-0.4244677702105224</v>
+        <v>-0.1769125694667655</v>
       </c>
       <c r="D131">
-        <v>0.3343534720161847</v>
+        <v>0.7319931058563364</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2423,13 +2663,13 @@
         <v>134</v>
       </c>
       <c r="B132">
-        <v>97.98883867345553</v>
+        <v>80.91828294799583</v>
       </c>
       <c r="C132">
-        <v>-0.4270219224289642</v>
+        <v>-0.1784215963300364</v>
       </c>
       <c r="D132">
-        <v>0.2345833906878618</v>
+        <v>0.07670204340249702</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2437,13 +2677,13 @@
         <v>135</v>
       </c>
       <c r="B133">
-        <v>98.90528262652728</v>
+        <v>81.4385467349785</v>
       </c>
       <c r="C133">
-        <v>-0.4403681935902031</v>
+        <v>-0.1859982534220168</v>
       </c>
       <c r="D133">
-        <v>0.4764156901916344</v>
+        <v>0.1418759647704181</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2451,13 +2691,13 @@
         <v>136</v>
       </c>
       <c r="B134">
-        <v>98.9071938677609</v>
+        <v>81.54494046635175</v>
       </c>
       <c r="C134">
-        <v>-0.4403960272004015</v>
+        <v>-0.1875476766944428</v>
       </c>
       <c r="D134">
-        <v>0.4214450787326763</v>
+        <v>0.1063482349010923</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2465,13 +2705,13 @@
         <v>137</v>
       </c>
       <c r="B135">
-        <v>99.78440721598638</v>
+        <v>81.5733624624034</v>
       </c>
       <c r="C135">
-        <v>-0.453170978873588</v>
+        <v>-0.1879615892583018</v>
       </c>
       <c r="D135">
-        <v>0.39745019283074</v>
+        <v>0.02448365544641497</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2479,13 +2719,13 @@
         <v>138</v>
       </c>
       <c r="B136">
-        <v>100.5960528126189</v>
+        <v>81.70222325461648</v>
       </c>
       <c r="C136">
-        <v>-0.4649910603779452</v>
+        <v>-0.1898382027371333</v>
       </c>
       <c r="D136">
-        <v>0.3818590852305652</v>
+        <v>0.1648050227775083</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2493,13 +2733,13 @@
         <v>139</v>
       </c>
       <c r="B137">
-        <v>101.8465453731726</v>
+        <v>82.39457954768551</v>
       </c>
       <c r="C137">
-        <v>-0.4832021170850378</v>
+        <v>-0.199921061374061</v>
       </c>
       <c r="D137">
-        <v>0.281332263746176</v>
+        <v>0.1474924304686204</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2507,13 +2747,13 @@
         <v>140</v>
       </c>
       <c r="B138">
-        <v>101.9263603600001</v>
+        <v>84.89786533478514</v>
       </c>
       <c r="C138">
-        <v>-0.4843644712621373</v>
+        <v>-0.2363766796327933</v>
       </c>
       <c r="D138">
-        <v>0.4315942109227289</v>
+        <v>0.1103243880336632</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2521,13 +2761,13 @@
         <v>141</v>
       </c>
       <c r="B139">
-        <v>102.5356608388521</v>
+        <v>85.58381225072721</v>
       </c>
       <c r="C139">
-        <v>-0.4932377792065841</v>
+        <v>-0.2463661978261242</v>
       </c>
       <c r="D139">
-        <v>0.3581241862918247</v>
+        <v>0.5991233778310178</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2535,13 +2775,13 @@
         <v>142</v>
       </c>
       <c r="B140">
-        <v>102.6489821655402</v>
+        <v>85.66687333479064</v>
       </c>
       <c r="C140">
-        <v>-0.4948880897894208</v>
+        <v>-0.2475758252639413</v>
       </c>
       <c r="D140">
-        <v>0.2736546186096283</v>
+        <v>0.1160707500643826</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2549,13 +2789,13 @@
         <v>143</v>
       </c>
       <c r="B141">
-        <v>103.7167484352416</v>
+        <v>85.78251485107938</v>
       </c>
       <c r="C141">
-        <v>-0.5104380840083724</v>
+        <v>-0.2492599250157193</v>
       </c>
       <c r="D141">
-        <v>0.4032122971732833</v>
+        <v>0.2566469433622143</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2563,13 +2803,13 @@
         <v>144</v>
       </c>
       <c r="B142">
-        <v>109.10531448363</v>
+        <v>86.82709156694065</v>
       </c>
       <c r="C142">
-        <v>-0.5889123468489803</v>
+        <v>-0.2644722072855434</v>
       </c>
       <c r="D142">
-        <v>0.2013501001529658</v>
+        <v>0.02674639247359616</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2577,13 +2817,13 @@
         <v>145</v>
       </c>
       <c r="B143">
-        <v>113.0410891823095</v>
+        <v>87.01850664548199</v>
       </c>
       <c r="C143">
-        <v>-0.6462294541113034</v>
+        <v>-0.2672598055167281</v>
       </c>
       <c r="D143">
-        <v>0.6076734712913363</v>
+        <v>0.01428537148615574</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2591,13 +2831,13 @@
         <v>146</v>
       </c>
       <c r="B144">
-        <v>113.1311693143717</v>
+        <v>87.02785486205696</v>
       </c>
       <c r="C144">
-        <v>-0.6475413006947335</v>
+        <v>-0.2673959445930625</v>
       </c>
       <c r="D144">
-        <v>0.2550565750037658</v>
+        <v>0.008859584317472918</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2605,13 +2845,13 @@
         <v>147</v>
       </c>
       <c r="B145">
-        <v>114.1128073371935</v>
+        <v>94.01262756916685</v>
       </c>
       <c r="C145">
-        <v>-0.6618370000562166</v>
+        <v>-0.3691159354733036</v>
       </c>
       <c r="D145">
-        <v>0.3529286285971286</v>
+        <v>0.1115121138368898</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2619,13 +2859,13 @@
         <v>148</v>
       </c>
       <c r="B146">
-        <v>115.8784210501392</v>
+        <v>94.62876210502735</v>
       </c>
       <c r="C146">
-        <v>-0.6875498211185316</v>
+        <v>-0.3780887685198158</v>
       </c>
       <c r="D146">
-        <v>0.4584372376317739</v>
+        <v>0.02967969138440198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup: Wed Jan  1 23:19:02 IST 2025
</commit_message>
<xml_diff>
--- a/linear_regression_with_significance.xlsx
+++ b/linear_regression_with_significance.xlsx
@@ -28,439 +28,439 @@
     <t>P-value</t>
   </si>
   <si>
+    <t>Temporal Fusiform Cortex, posterior division Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Change</t>
+  </si>
+  <si>
+    <t>Temporal Pole Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Change</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Change</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Avg</t>
+  </si>
+  <si>
+    <t>Precuneous Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cingulate Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Paracingulate Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Subcallosal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Angular Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Supramarginal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Orbital Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Parietal Lobule Volume Change</t>
+  </si>
+  <si>
+    <t>Postcentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Precentral Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
+  </si>
+  <si>
+    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Frontal Gyrus Volume Change</t>
+  </si>
+  <si>
+    <t>Insular Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Temporale Volume Avg</t>
+  </si>
+  <si>
+    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
+  </si>
+  <si>
+    <t>Planum Polare Volume Avg</t>
+  </si>
+  <si>
+    <t>Parietal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Central Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Frontal Opercular Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Occipital Fusiform Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Lingual Gyrus Volume Avg</t>
+  </si>
+  <si>
+    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Cuneal Cortex Change</t>
+  </si>
+  <si>
+    <t>Frontal Pole Change</t>
+  </si>
+  <si>
+    <t>Intracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Occipital Pole Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age at baseline </t>
+  </si>
+  <si>
+    <t>Occipital Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Supracalcarine Cortex Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Pole Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Medial Cortex Volume Change</t>
+  </si>
+  <si>
+    <t>Frontal Pole Volume Change</t>
+  </si>
+  <si>
     <t>Frontal Pole Volume Avg</t>
   </si>
   <si>
-    <t>Supramarginal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Avg</t>
+    <t>Temporal Pole Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
+  </si>
+  <si>
+    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
   </si>
   <si>
     <t>Inferior Temporal Gyrus, anterior division Volume Avg</t>
   </si>
   <si>
-    <t>Superior Parietal Lobule Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Polare Volume Change</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Temporale Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Insular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Volume Change</t>
-  </si>
-  <si>
-    <t>Temporal Pole Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Parahippocampal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Volume Avg</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Intracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars triangularis Change</t>
-  </si>
-  <si>
-    <t>Occipital Pole Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Volume Change</t>
-  </si>
-  <si>
-    <t>Lingual Gyrus Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Avg</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Occipital Pole Volume Avg</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Volume Avg</t>
-  </si>
-  <si>
-    <t>Planum Polare Change</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex Change</t>
-  </si>
-  <si>
     <t>Inferior Temporal Gyrus, anterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Heschl's Gyrus (includes H1 and H2) Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Volume Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Subcallosal Cortex Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, anterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Volume Change</t>
-  </si>
-  <si>
-    <t>Planum Temporale Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Superior Temporal Gyrus, posterior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Postcentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Cuneal Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Medial Cortex Change</t>
-  </si>
-  <si>
-    <t>Insular Cortex Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Volume Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Volume Change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age at baseline </t>
-  </si>
-  <si>
-    <t>Occipital Fusiform Gyrus Change</t>
-  </si>
-  <si>
-    <t>Frontal Orbital Cortex Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Volume Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Volume Change</t>
-  </si>
-  <si>
-    <t>Supracalcarine Cortex Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Precentral Gyrus Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Superior Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Gyrus, pars opercularis Change</t>
-  </si>
-  <si>
-    <t>Middle Temporal Gyrus, temporooccipital part Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, inferior division Volume Avg</t>
-  </si>
-  <si>
-    <t>Frontal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Parietal Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Temporal Fusiform Cortex, anterior division Change</t>
-  </si>
-  <si>
-    <t>Inferior Temporal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Cingulate Gyrus, anterior division Change</t>
-  </si>
-  <si>
-    <t>Central Opercular Cortex Change</t>
-  </si>
-  <si>
-    <t>Precuneous Cortex Change</t>
-  </si>
-  <si>
-    <t>Frontal Pole Change</t>
-  </si>
-  <si>
-    <t>Juxtapositional Lobule Cortex (formerly Supplementary Motor Cortex) Change</t>
-  </si>
-  <si>
-    <t>Paracingulate Gyrus Change</t>
-  </si>
-  <si>
-    <t>Superior Parietal Lobule Change</t>
-  </si>
-  <si>
-    <t>Supramarginal Gyrus, posterior division Change</t>
-  </si>
-  <si>
-    <t>Middle Frontal Gyrus Change</t>
-  </si>
-  <si>
-    <t>Lateral Occipital Cortex, superior division Change</t>
-  </si>
-  <si>
-    <t>Angular Gyrus Change</t>
   </si>
 </sst>
 </file>
@@ -843,13 +843,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>55.54202081773011</v>
+        <v>43.82964001918847</v>
       </c>
       <c r="C2">
-        <v>0.1911356191592701</v>
+        <v>0.3617042715652163</v>
       </c>
       <c r="D2">
-        <v>0.05279187603332048</v>
+        <v>0.003882332744808361</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -857,13 +857,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>60.41752672616147</v>
+        <v>50.27256518816761</v>
       </c>
       <c r="C3">
-        <v>0.1201331059296874</v>
+        <v>0.2678752642499862</v>
       </c>
       <c r="D3">
-        <v>0.06112447544471123</v>
+        <v>0.00460519954801258</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -871,13 +871,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>61.07141577331057</v>
+        <v>51.21334452291418</v>
       </c>
       <c r="C4">
-        <v>0.1106104499032442</v>
+        <v>0.2541745943264926</v>
       </c>
       <c r="D4">
-        <v>0.05287306437930851</v>
+        <v>0.004235346921290491</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -885,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>63.4655907086429</v>
+        <v>51.32953773399369</v>
       </c>
       <c r="C5">
-        <v>0.07574382463141416</v>
+        <v>0.252482460184558</v>
       </c>
       <c r="D5">
-        <v>0.2239066625532428</v>
+        <v>0.01370050952506687</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -899,13 +899,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>64.52744180229787</v>
+        <v>51.77270546811044</v>
       </c>
       <c r="C6">
-        <v>0.06027997375294358</v>
+        <v>0.2460285611440228</v>
       </c>
       <c r="D6">
-        <v>0.2762699270416408</v>
+        <v>0.007951519736736374</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -913,13 +913,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>64.8906118629907</v>
+        <v>52.24500947924039</v>
       </c>
       <c r="C7">
-        <v>0.05499108937392194</v>
+        <v>0.239150347389703</v>
       </c>
       <c r="D7">
-        <v>0.2326623324699504</v>
+        <v>0.01390325209691019</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -927,13 +927,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>64.94838171743879</v>
+        <v>52.39111547385767</v>
       </c>
       <c r="C8">
-        <v>0.05414978081399813</v>
+        <v>0.2370225901865388</v>
       </c>
       <c r="D8">
-        <v>0.2204292672352802</v>
+        <v>0.02020394565701578</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -941,13 +941,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>65.62484253401277</v>
+        <v>52.79747503553556</v>
       </c>
       <c r="C9">
-        <v>0.04429840969884302</v>
+        <v>0.2311047324922006</v>
       </c>
       <c r="D9">
-        <v>0.06122981799759784</v>
+        <v>0.03156294400790094</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -955,13 +955,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>66.6513888254446</v>
+        <v>52.84811716862946</v>
       </c>
       <c r="C10">
-        <v>0.0293487064255642</v>
+        <v>0.2303672256995709</v>
       </c>
       <c r="D10">
-        <v>0.2396312773643319</v>
+        <v>0.01827745667871282</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -969,13 +969,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>67.22290084466719</v>
+        <v>53.0462959516558</v>
       </c>
       <c r="C11">
-        <v>0.0210257158543613</v>
+        <v>0.227481126917634</v>
       </c>
       <c r="D11">
-        <v>0.3590941830306501</v>
+        <v>0.01837256215316668</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -983,13 +983,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>67.4183338034219</v>
+        <v>53.24490850081902</v>
       </c>
       <c r="C12">
-        <v>0.0181796048045354</v>
+        <v>0.2245887111531212</v>
       </c>
       <c r="D12">
-        <v>0.3843822982127002</v>
+        <v>0.01623753940426115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -997,13 +997,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>67.51205211794567</v>
+        <v>54.08759779331723</v>
       </c>
       <c r="C13">
-        <v>0.01681477498137363</v>
+        <v>0.2123165369905258</v>
       </c>
       <c r="D13">
-        <v>0.4056856226221157</v>
+        <v>0.00800091219450047</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1011,13 +1011,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>67.59410185777965</v>
+        <v>54.42247822450501</v>
       </c>
       <c r="C14">
-        <v>0.01561987585757796</v>
+        <v>0.2074396375072086</v>
       </c>
       <c r="D14">
-        <v>0.4447907238901564</v>
+        <v>0.01726995635061003</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1025,13 +1025,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>67.80414079965385</v>
+        <v>54.79309884243684</v>
       </c>
       <c r="C15">
-        <v>0.01256105631572058</v>
+        <v>0.2020422498674246</v>
       </c>
       <c r="D15">
-        <v>0.550651527199203</v>
+        <v>0.01581537858864748</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1039,13 +1039,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>68.02061569407579</v>
+        <v>55.18175892848411</v>
       </c>
       <c r="C16">
-        <v>0.00940850930957593</v>
+        <v>0.1963821515269304</v>
       </c>
       <c r="D16">
-        <v>0.4684520375045017</v>
+        <v>0.02058224528221539</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1053,13 +1053,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>68.21686793519677</v>
+        <v>55.34022654811989</v>
       </c>
       <c r="C17">
-        <v>0.006550466963153756</v>
+        <v>0.1940743706584482</v>
       </c>
       <c r="D17">
-        <v>0.5507431244906833</v>
+        <v>0.01590106009418793</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1067,13 +1067,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>68.25051687217841</v>
+        <v>55.37393588116091</v>
       </c>
       <c r="C18">
-        <v>0.00606043390031441</v>
+        <v>0.193583458041346</v>
       </c>
       <c r="D18">
-        <v>0.590012499156545</v>
+        <v>0.01535273290715243</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1081,13 +1081,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>68.32098716091679</v>
+        <v>55.47096386607953</v>
       </c>
       <c r="C19">
-        <v>0.005034167559464398</v>
+        <v>0.1921704291347642</v>
       </c>
       <c r="D19">
-        <v>0.4025143907045666</v>
+        <v>0.009395484915043028</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1095,13 +1095,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>68.38071128778341</v>
+        <v>55.4757891732641</v>
       </c>
       <c r="C20">
-        <v>0.004164398721600904</v>
+        <v>0.1921001576709112</v>
       </c>
       <c r="D20">
-        <v>0.5865971475663934</v>
+        <v>0.01223826059889141</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1109,13 +1109,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>68.47809290147293</v>
+        <v>55.48553596988729</v>
       </c>
       <c r="C21">
-        <v>0.002746219881462175</v>
+        <v>0.1919582140307676</v>
       </c>
       <c r="D21">
-        <v>0.6100421788994763</v>
+        <v>0.008491428474159774</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1123,13 +1123,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>68.49987697929187</v>
+        <v>55.55647117056346</v>
       </c>
       <c r="C22">
-        <v>0.002428976029730023</v>
+        <v>0.1909251771277167</v>
       </c>
       <c r="D22">
-        <v>0.5353861247105034</v>
+        <v>0.003358438696923644</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1137,13 +1137,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>68.54771342131046</v>
+        <v>55.8520084537104</v>
       </c>
       <c r="C23">
-        <v>0.001732328815866935</v>
+        <v>0.1866212361110134</v>
       </c>
       <c r="D23">
-        <v>0.6017612687645815</v>
+        <v>0.008906301830053651</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1151,13 +1151,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>68.67177649513013</v>
+        <v>55.94262972391375</v>
       </c>
       <c r="C24">
-        <v>-7.441497762328275E-05</v>
+        <v>0.1853015088750425</v>
       </c>
       <c r="D24">
-        <v>0.3221087969052605</v>
+        <v>0.01691999994869852</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1165,13 +1165,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>68.83043204145818</v>
+        <v>56.17399873574797</v>
       </c>
       <c r="C25">
-        <v>-0.002384932642594872</v>
+        <v>0.1819320572463887</v>
       </c>
       <c r="D25">
-        <v>0.6343160103450627</v>
+        <v>0.007273627939610533</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1179,13 +1179,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>69.00943452746645</v>
+        <v>56.24314928982295</v>
       </c>
       <c r="C26">
-        <v>-0.004991764963103718</v>
+        <v>0.1809250103423842</v>
       </c>
       <c r="D26">
-        <v>0.8076779085040482</v>
+        <v>0.02133519164801764</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1193,13 +1193,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>69.04182505902726</v>
+        <v>57.09232671126805</v>
       </c>
       <c r="C27">
-        <v>-0.005463471733406777</v>
+        <v>0.1685583488650284</v>
       </c>
       <c r="D27">
-        <v>0.6210298847256009</v>
+        <v>0.01395379724622524</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1207,13 +1207,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>69.05964728042945</v>
+        <v>57.35078205357963</v>
       </c>
       <c r="C28">
-        <v>-0.005723018647030731</v>
+        <v>0.164794436112918</v>
       </c>
       <c r="D28">
-        <v>0.7630940607759764</v>
+        <v>0.01322562920544901</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1221,13 +1221,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>69.08496481839377</v>
+        <v>57.47217468437834</v>
       </c>
       <c r="C29">
-        <v>-0.006091720656220101</v>
+        <v>0.1630265822663349</v>
       </c>
       <c r="D29">
-        <v>0.5476313920376215</v>
+        <v>0.01170904274596512</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1235,13 +1235,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>69.18168494670948</v>
+        <v>57.62862815564284</v>
       </c>
       <c r="C30">
-        <v>-0.007500266214215845</v>
+        <v>0.1607481336556869</v>
       </c>
       <c r="D30">
-        <v>0.8100519433945763</v>
+        <v>0.03452629303765548</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1249,13 +1249,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>69.18857660246675</v>
+        <v>57.67694746897299</v>
       </c>
       <c r="C31">
-        <v>-0.007600630133011155</v>
+        <v>0.1600444543353449</v>
       </c>
       <c r="D31">
-        <v>0.7352002814750809</v>
+        <v>0.02032190865117174</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1263,13 +1263,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>69.21633982466746</v>
+        <v>57.93972264995686</v>
       </c>
       <c r="C32">
-        <v>-0.008004948902924136</v>
+        <v>0.1562176313113078</v>
       </c>
       <c r="D32">
-        <v>0.03562289372370342</v>
+        <v>0.04073731721260194</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1277,13 +1277,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>69.29651490988087</v>
+        <v>58.2754881485109</v>
       </c>
       <c r="C33">
-        <v>-0.009172547231274919</v>
+        <v>0.1513278424974142</v>
       </c>
       <c r="D33">
-        <v>0.4087193821993432</v>
+        <v>0.009237688091861755</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1291,13 +1291,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>69.30006141437428</v>
+        <v>58.65661692333895</v>
       </c>
       <c r="C34">
-        <v>-0.009224195354965437</v>
+        <v>0.1457774234465201</v>
       </c>
       <c r="D34">
-        <v>0.4388105046984263</v>
+        <v>0.03682842092746497</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1305,13 +1305,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>69.34298140836728</v>
+        <v>59.73198369141307</v>
       </c>
       <c r="C35">
-        <v>-0.009849243811173913</v>
+        <v>0.1301167423580621</v>
       </c>
       <c r="D35">
-        <v>0.8751914167575987</v>
+        <v>0.02768909672531274</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1319,13 +1319,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>69.39469920510095</v>
+        <v>59.8117319703845</v>
       </c>
       <c r="C36">
-        <v>-0.01060241560826625</v>
+        <v>0.1289553596545947</v>
       </c>
       <c r="D36">
-        <v>0.998948466201195</v>
+        <v>0.05384909259798484</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1333,13 +1333,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>69.44168618555629</v>
+        <v>59.91481209692797</v>
       </c>
       <c r="C37">
-        <v>-0.01128669202266441</v>
+        <v>0.1274541927631849</v>
       </c>
       <c r="D37">
-        <v>0.9461287414802102</v>
+        <v>0.04774671909658303</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1347,13 +1347,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>69.53708624176514</v>
+        <v>60.19689130902832</v>
       </c>
       <c r="C38">
-        <v>-0.01267601322958933</v>
+        <v>0.1233462430724031</v>
       </c>
       <c r="D38">
-        <v>0.1597869090806618</v>
+        <v>0.02650096610662288</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1361,13 +1361,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>69.61708791345816</v>
+        <v>60.47134657107444</v>
       </c>
       <c r="C39">
-        <v>-0.01384108611832269</v>
+        <v>0.1193493217804693</v>
       </c>
       <c r="D39">
-        <v>0.9566496111225951</v>
+        <v>0.01184432518946184</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1375,13 +1375,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>69.73305765982361</v>
+        <v>61.62713368880421</v>
       </c>
       <c r="C40">
-        <v>-0.01552996591976141</v>
+        <v>0.102517470551395</v>
       </c>
       <c r="D40">
-        <v>0.498124836369502</v>
+        <v>0.03634026854406287</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1389,13 +1389,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>69.82921431641626</v>
+        <v>62.29698429138788</v>
       </c>
       <c r="C41">
-        <v>-0.01693030557887742</v>
+        <v>0.09276236468852594</v>
       </c>
       <c r="D41">
-        <v>0.9101854880917394</v>
+        <v>0.1664547747723916</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1403,13 +1403,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>69.83195989077272</v>
+        <v>62.61172112579162</v>
       </c>
       <c r="C42">
-        <v>-0.01697028967144742</v>
+        <v>0.08817881855643273</v>
       </c>
       <c r="D42">
-        <v>0.9305282233166774</v>
+        <v>0.015711090886546</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1417,13 +1417,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>69.85046687938711</v>
+        <v>63.54580519146118</v>
       </c>
       <c r="C43">
-        <v>-0.01723980892311339</v>
+        <v>0.07457565255153631</v>
       </c>
       <c r="D43">
-        <v>0.5254703628853179</v>
+        <v>0.02309120680282317</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1431,13 +1431,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>69.85688532454452</v>
+        <v>64.71046712749802</v>
       </c>
       <c r="C44">
-        <v>-0.01733328142540547</v>
+        <v>0.05761455639565993</v>
       </c>
       <c r="D44">
-        <v>0.8364136660964817</v>
+        <v>0.06523224204751547</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1445,13 +1445,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>69.86544975791065</v>
+        <v>67.36339097623663</v>
       </c>
       <c r="C45">
-        <v>-0.01745800618316484</v>
+        <v>0.01897974306451522</v>
       </c>
       <c r="D45">
-        <v>0.490852013882599</v>
+        <v>0.2323104262338641</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1459,13 +1459,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>69.88207352119618</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C46">
-        <v>-0.01770009982324527</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D46">
-        <v>0.5270967494510257</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1473,13 +1473,13 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>70.02863807811531</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C47">
-        <v>-0.01983453511818412</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D47">
-        <v>0.8895010247528776</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1487,13 +1487,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>70.08901580320889</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C48">
-        <v>-0.02071382237682862</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D48">
-        <v>0.8406279839112907</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1501,13 +1501,13 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>70.17031557141169</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C49">
-        <v>-0.02189779958366556</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D49">
-        <v>0.5724729481208475</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1515,13 +1515,13 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>70.22515261390623</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C50">
-        <v>-0.02269639728989659</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D50">
-        <v>0.9724700730256017</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1529,13 +1529,13 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>70.24960434154804</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C51">
-        <v>-0.02305249041089374</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D51">
-        <v>0.6731288165574267</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1543,13 +1543,13 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>70.31389504475381</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C52">
-        <v>-0.02398876278767692</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D52">
-        <v>0.7130037887185959</v>
+        <v>0.02560846533537106</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1557,13 +1557,13 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>70.41351154870434</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C53">
-        <v>-0.0254394885733642</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D53">
-        <v>0.752997486680917</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1571,13 +1571,13 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>70.62662373793543</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C54">
-        <v>-0.02854306414469088</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D54">
-        <v>0.5959985032632197</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1585,13 +1585,13 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>70.72061079274492</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C55">
-        <v>-0.02991180766133383</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D55">
-        <v>0.03800878798105314</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1599,13 +1599,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>70.77893538931397</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C56">
-        <v>-0.03076119499000929</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D56">
-        <v>0.6992242603346432</v>
+        <v>0.02554098979904919</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1613,13 +1613,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>70.98905848622871</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C57">
-        <v>-0.03382124009070941</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D57">
-        <v>0.6288256261527839</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1627,13 +1627,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>71.18149853399399</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C58">
-        <v>-0.03662376505816489</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D58">
-        <v>0.771664349340643</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1641,13 +1641,13 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>71.20807043654648</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C59">
-        <v>-0.03701073451281278</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D59">
-        <v>0.6542874573175916</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1655,13 +1655,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>71.21537666730381</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C60">
-        <v>-0.03711713593160915</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D60">
-        <v>0.07780434642915535</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1669,13 +1669,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>71.22643447325102</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C61">
-        <v>-0.03727817194054883</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D61">
-        <v>0.1145759339875331</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1683,13 +1683,13 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>71.23482563851836</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C62">
-        <v>-0.03740037337648094</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D62">
-        <v>0.1163006391407411</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1697,13 +1697,13 @@
         <v>65</v>
       </c>
       <c r="B63">
-        <v>71.62458447463652</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C63">
-        <v>-0.04307647293159977</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D63">
-        <v>0.4182516193871859</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1711,13 +1711,13 @@
         <v>66</v>
       </c>
       <c r="B64">
-        <v>71.76354420803904</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C64">
-        <v>-0.04510015836950054</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D64">
-        <v>0.2590674548641074</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1725,13 +1725,13 @@
         <v>67</v>
       </c>
       <c r="B65">
-        <v>72.03860874525633</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C65">
-        <v>-0.04910595260082018</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D65">
-        <v>0.7741005029983061</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1739,13 +1739,13 @@
         <v>68</v>
       </c>
       <c r="B66">
-        <v>72.05383022115026</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C66">
-        <v>-0.04932762457985818</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D66">
-        <v>0.6159789939789663</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1753,13 +1753,13 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <v>72.05620902818163</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C67">
-        <v>-0.04936226740070349</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D67">
-        <v>0.545905277550076</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1767,13 +1767,13 @@
         <v>70</v>
       </c>
       <c r="B68">
-        <v>72.19097971272089</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C68">
-        <v>-0.05132494727263448</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D68">
-        <v>0.3948316531874997</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1781,13 +1781,13 @@
         <v>71</v>
       </c>
       <c r="B69">
-        <v>72.19565574624463</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C69">
-        <v>-0.05139304484822271</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D69">
-        <v>0.05224086509107263</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1795,13 +1795,13 @@
         <v>72</v>
       </c>
       <c r="B70">
-        <v>72.27261253158173</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C70">
-        <v>-0.05251377473177254</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D70">
-        <v>0.3683686240214875</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1809,13 +1809,13 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>72.4789438928867</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C71">
-        <v>-0.05551860038184531</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D71">
-        <v>0.4843417897480464</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1823,13 +1823,13 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>72.50071887577786</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C72">
-        <v>-0.05583571178317293</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D72">
-        <v>0.05714288744451292</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1837,13 +1837,13 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>72.65361118593795</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C73">
-        <v>-0.05806229882433911</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D73">
-        <v>0.6272481590341763</v>
+        <v>0.02554098979904942</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1851,13 +1851,13 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>72.68513033785204</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C74">
-        <v>-0.05852131559978702</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D74">
-        <v>0.6719229031495553</v>
+        <v>0.02554098979904898</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1865,13 +1865,13 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>72.70463798734139</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C75">
-        <v>-0.05880540758264141</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D75">
-        <v>0.1963047371919701</v>
+        <v>0.02554098979904919</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1879,13 +1879,13 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>72.76544338441994</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C76">
-        <v>-0.05969092307407697</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D76">
-        <v>0.821733778338277</v>
+        <v>0.02554098979904919</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1893,13 +1893,13 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>72.8750271996623</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C77">
-        <v>-0.06128680387857721</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D77">
-        <v>0.319199545339699</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1907,13 +1907,13 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>72.90094087057615</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C78">
-        <v>-0.061664187435575</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D78">
-        <v>0.00887383526854609</v>
+        <v>0.02554098979904923</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1921,13 +1921,13 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>73.10580274306524</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C79">
-        <v>-0.06464761276308617</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D79">
-        <v>0.5360903821672427</v>
+        <v>0.02554098979904926</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1935,13 +1935,13 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>73.11216917677024</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C80">
-        <v>-0.0647403278170422</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D80">
-        <v>0.4228408208636953</v>
+        <v>0.02554098979905135</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1949,13 +1949,13 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>73.12103271424225</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C81">
-        <v>-0.06486940845983846</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D81">
-        <v>0.1174649469213347</v>
+        <v>0.02554098979904948</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1963,13 +1963,13 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>73.161147110032</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C82">
-        <v>-0.06545359868978662</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D82">
-        <v>0.1251405111592915</v>
+        <v>0.02554098979904952</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1977,13 +1977,13 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>73.2931638878888</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C83">
-        <v>-0.0673761731245941</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D83">
-        <v>0.9702461192060646</v>
+        <v>0.02554098979904962</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1991,13 +1991,13 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>73.29696890749015</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C84">
-        <v>-0.06743158603141008</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D84">
-        <v>0.101888757366417</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2005,13 +2005,13 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>73.60071087226467</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C85">
-        <v>-0.07185501270288364</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D85">
-        <v>0.4918852215887154</v>
+        <v>0.02554098979904923</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2019,13 +2019,13 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>73.65913795511882</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C86">
-        <v>-0.07270589255027415</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D86">
-        <v>0.162323728445789</v>
+        <v>0.02554098979904926</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2033,13 +2033,13 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>73.7104171550109</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C87">
-        <v>-0.07345267701472191</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D87">
-        <v>0.7751121850913547</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2047,13 +2047,13 @@
         <v>90</v>
       </c>
       <c r="B88">
-        <v>73.71316207677627</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C88">
-        <v>-0.07349265160353791</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D88">
-        <v>0.1326884892573001</v>
+        <v>0.02554098979904923</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2061,13 +2061,13 @@
         <v>91</v>
       </c>
       <c r="B89">
-        <v>73.98451824771466</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C89">
-        <v>-0.07744444050069887</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D89">
-        <v>0.4296481439261044</v>
+        <v>0.02554098979904962</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2075,13 +2075,13 @@
         <v>92</v>
       </c>
       <c r="B90">
-        <v>74.0626337073423</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C90">
-        <v>-0.07858204428168403</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D90">
-        <v>0.497459911239897</v>
+        <v>0.02554098979904948</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2089,13 +2089,13 @@
         <v>93</v>
       </c>
       <c r="B91">
-        <v>74.13199491456501</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C91">
-        <v>-0.07959215894997596</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D91">
-        <v>0.5291293396105173</v>
+        <v>0.0255409897990493</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2103,13 +2103,13 @@
         <v>94</v>
       </c>
       <c r="B92">
-        <v>74.13259831064728</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C92">
-        <v>-0.07960094627156233</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D92">
-        <v>0.13844047464105</v>
+        <v>0.02554098979904932</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2117,13 +2117,13 @@
         <v>95</v>
       </c>
       <c r="B93">
-        <v>74.30647085706134</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C93">
-        <v>-0.08213307073390297</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D93">
-        <v>0.3874311337441763</v>
+        <v>0.02554098979904944</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2131,13 +2131,13 @@
         <v>96</v>
       </c>
       <c r="B94">
-        <v>74.61859849209365</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C94">
-        <v>-0.08667861881689776</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D94">
-        <v>0.8976683566818522</v>
+        <v>0.02554098979904904</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2145,13 +2145,13 @@
         <v>97</v>
       </c>
       <c r="B95">
-        <v>74.89313439566257</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C95">
-        <v>-0.09067671449994053</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D95">
-        <v>0.2950987867948573</v>
+        <v>0.02554098979904926</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2159,13 +2159,13 @@
         <v>98</v>
       </c>
       <c r="B96">
-        <v>74.91723805327581</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C96">
-        <v>-0.09102773863993896</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D96">
-        <v>0.9278424656488063</v>
+        <v>0.02554098979904952</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2173,13 +2173,13 @@
         <v>99</v>
       </c>
       <c r="B97">
-        <v>75.16934553405025</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C97">
-        <v>-0.09469920680655708</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D97">
-        <v>0.1111094374854422</v>
+        <v>0.02554098979904951</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2187,13 +2187,13 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>75.26856224306069</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C98">
-        <v>-0.09614411033583536</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D98">
-        <v>0.09226146958348402</v>
+        <v>0.02554098979904937</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2201,13 +2201,13 @@
         <v>101</v>
       </c>
       <c r="B99">
-        <v>75.29235353433367</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C99">
-        <v>-0.09649058545146127</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D99">
-        <v>0.3409550655347707</v>
+        <v>0.02554098979904932</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2215,13 +2215,13 @@
         <v>102</v>
       </c>
       <c r="B100">
-        <v>75.34077379563284</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C100">
-        <v>-0.09719573488785693</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D100">
-        <v>0.2186456991050574</v>
+        <v>0.02554098979904952</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2229,13 +2229,13 @@
         <v>103</v>
       </c>
       <c r="B101">
-        <v>75.43389954537813</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C101">
-        <v>-0.098551935126866</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D101">
-        <v>0.6436681146391308</v>
+        <v>0.0256084653353712</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2243,13 +2243,13 @@
         <v>104</v>
       </c>
       <c r="B102">
-        <v>75.48258320289968</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C102">
-        <v>-0.09926092043057788</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D102">
-        <v>0.1328872130873812</v>
+        <v>0.02554098979904944</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2257,13 +2257,13 @@
         <v>105</v>
       </c>
       <c r="B103">
-        <v>75.52293937361105</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C103">
-        <v>-0.09984863165452995</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D103">
-        <v>0.1317736248989538</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2271,13 +2271,13 @@
         <v>106</v>
       </c>
       <c r="B104">
-        <v>75.60148324056735</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C104">
-        <v>-0.1009924743771944</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D104">
-        <v>0.2092419325749682</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2285,13 +2285,13 @@
         <v>107</v>
       </c>
       <c r="B105">
-        <v>75.74154818583737</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C105">
-        <v>-0.1030322551335541</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D105">
-        <v>0.4923645278197668</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2299,13 +2299,13 @@
         <v>108</v>
       </c>
       <c r="B106">
-        <v>75.75911344173647</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C106">
-        <v>-0.1032880598311139</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D106">
-        <v>0.1285763626914587</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2313,13 +2313,13 @@
         <v>109</v>
       </c>
       <c r="B107">
-        <v>75.96721543141253</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C107">
-        <v>-0.1063186713312505</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D107">
-        <v>0.369190355059335</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2327,13 +2327,13 @@
         <v>110</v>
       </c>
       <c r="B108">
-        <v>76.22290216397577</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C108">
-        <v>-0.110042264523919</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D108">
-        <v>0.149798050528452</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2341,13 +2341,13 @@
         <v>111</v>
       </c>
       <c r="B109">
-        <v>76.49084418670549</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C109">
-        <v>-0.1139443328160994</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D109">
-        <v>0.04203691712059767</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2355,13 +2355,13 @@
         <v>112</v>
       </c>
       <c r="B110">
-        <v>76.57821785601229</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C110">
-        <v>-0.1152167648933828</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D110">
-        <v>0.551297681181437</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2369,13 +2369,13 @@
         <v>113</v>
       </c>
       <c r="B111">
-        <v>76.64224804114292</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C111">
-        <v>-0.1161492433176154</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D111">
-        <v>0.009220522230884928</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2383,13 +2383,13 @@
         <v>114</v>
       </c>
       <c r="B112">
-        <v>76.93326986368164</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C112">
-        <v>-0.1203874251992472</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D112">
-        <v>0.153421811511493</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2397,13 +2397,13 @@
         <v>115</v>
       </c>
       <c r="B113">
-        <v>77.35496289372983</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C113">
-        <v>-0.126528585831017</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D113">
-        <v>0.157033176695222</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2411,13 +2411,13 @@
         <v>116</v>
       </c>
       <c r="B114">
-        <v>77.40178075804917</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C114">
-        <v>-0.1272103993890656</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D114">
-        <v>0.9541721462265929</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2425,13 +2425,13 @@
         <v>117</v>
       </c>
       <c r="B115">
-        <v>77.51011673093114</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C115">
-        <v>-0.128788107732007</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D115">
-        <v>0.2200283506934367</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2439,13 +2439,13 @@
         <v>118</v>
       </c>
       <c r="B116">
-        <v>77.61976330583501</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C116">
-        <v>-0.1303849025121604</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D116">
-        <v>0.005412367384066267</v>
+        <v>0.02554098979905188</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2453,13 +2453,13 @@
         <v>119</v>
       </c>
       <c r="B117">
-        <v>77.67216964458771</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C117">
-        <v>-0.1311481016202094</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D117">
-        <v>0.8794862275341265</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2467,13 +2467,13 @@
         <v>120</v>
       </c>
       <c r="B118">
-        <v>78.04832652780568</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C118">
-        <v>-0.1366261144826071</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D118">
-        <v>0.1993894770059438</v>
+        <v>0.02554098979904909</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2481,13 +2481,13 @@
         <v>121</v>
       </c>
       <c r="B119">
-        <v>78.21566079056869</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C119">
-        <v>-0.1390630212218742</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D119">
-        <v>0.2128049735853601</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2495,13 +2495,13 @@
         <v>122</v>
       </c>
       <c r="B120">
-        <v>78.29536958931622</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C120">
-        <v>-0.1402238289706246</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D120">
-        <v>0.1459243744122649</v>
+        <v>0.02554098979904913</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2509,13 +2509,13 @@
         <v>123</v>
       </c>
       <c r="B121">
-        <v>78.3716102651304</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C121">
-        <v>-0.1413341300747144</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D121">
-        <v>0.092990422424097</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2523,13 +2523,13 @@
         <v>124</v>
       </c>
       <c r="B122">
-        <v>78.57220955481699</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C122">
-        <v>-0.1442554789536457</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D122">
-        <v>0.3349481713517459</v>
+        <v>0.02554098979904912</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2537,13 +2537,13 @@
         <v>125</v>
       </c>
       <c r="B123">
-        <v>78.78344687676518</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C123">
-        <v>-0.1473317506325027</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D123">
-        <v>0.453334142204731</v>
+        <v>0.02554098979904957</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2551,13 +2551,13 @@
         <v>126</v>
       </c>
       <c r="B124">
-        <v>78.84672576799851</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C124">
-        <v>-0.1482532878834733</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D124">
-        <v>0.1034381434860657</v>
+        <v>0.02554098979904926</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2565,13 +2565,13 @@
         <v>127</v>
       </c>
       <c r="B125">
-        <v>79.11268053108718</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C125">
-        <v>-0.1521264155012696</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D125">
-        <v>0.02270697528117758</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2579,13 +2579,13 @@
         <v>128</v>
       </c>
       <c r="B126">
-        <v>79.35480458316975</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C126">
-        <v>-0.1556524939296566</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D126">
-        <v>0.06867740949709193</v>
+        <v>0.02554098979904915</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2593,13 +2593,13 @@
         <v>129</v>
       </c>
       <c r="B127">
-        <v>79.82782480083107</v>
+        <v>69.24058769513314</v>
       </c>
       <c r="C127">
-        <v>-0.1625411378761805</v>
+        <v>-0.008358073230094298</v>
       </c>
       <c r="D127">
-        <v>0.02750431193371585</v>
+        <v>0.02554098979904922</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2607,13 +2607,13 @@
         <v>130</v>
       </c>
       <c r="B128">
-        <v>80.51115142493498</v>
+        <v>69.24374132719311</v>
       </c>
       <c r="C128">
-        <v>-0.1724924964796355</v>
+        <v>-0.008403999910579163</v>
       </c>
       <c r="D128">
-        <v>0.04173361010978927</v>
+        <v>0.06377312273760571</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2621,13 +2621,13 @@
         <v>131</v>
       </c>
       <c r="B129">
-        <v>80.58956048240258</v>
+        <v>69.31515365509853</v>
       </c>
       <c r="C129">
-        <v>-0.1736343759573191</v>
+        <v>-0.009443985268425159</v>
       </c>
       <c r="D129">
-        <v>0.1419051958502771</v>
+        <v>0.02298376423891035</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2635,13 +2635,13 @@
         <v>132</v>
       </c>
       <c r="B130">
-        <v>80.71984632715981</v>
+        <v>70.09793950314105</v>
       </c>
       <c r="C130">
-        <v>-0.175531742628541</v>
+        <v>-0.02084377917195712</v>
       </c>
       <c r="D130">
-        <v>0.05900138443219891</v>
+        <v>0.06632289324755807</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2649,13 +2649,13 @@
         <v>133</v>
       </c>
       <c r="B131">
-        <v>80.81466310338456</v>
+        <v>75.51812461807199</v>
       </c>
       <c r="C131">
-        <v>-0.1769125694667655</v>
+        <v>-0.09977851385541725</v>
       </c>
       <c r="D131">
-        <v>0.7319931058563364</v>
+        <v>0.09518650699452047</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2663,13 +2663,13 @@
         <v>134</v>
       </c>
       <c r="B132">
-        <v>80.91828294799583</v>
+        <v>78.04832652780568</v>
       </c>
       <c r="C132">
-        <v>-0.1784215963300364</v>
+        <v>-0.1366261144826071</v>
       </c>
       <c r="D132">
-        <v>0.07670204340249702</v>
+        <v>0.1993894770059438</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2677,13 +2677,13 @@
         <v>135</v>
       </c>
       <c r="B133">
-        <v>81.4385467349785</v>
+        <v>82.18647789671594</v>
       </c>
       <c r="C133">
-        <v>-0.1859982534220168</v>
+        <v>-0.1968904548065429</v>
       </c>
       <c r="D133">
-        <v>0.1418759647704181</v>
+        <v>0.05506596214507239</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2691,13 +2691,13 @@
         <v>136</v>
       </c>
       <c r="B134">
-        <v>81.54494046635175</v>
+        <v>83.85911834609003</v>
       </c>
       <c r="C134">
-        <v>-0.1875476766944428</v>
+        <v>-0.2212492963022819</v>
       </c>
       <c r="D134">
-        <v>0.1063482349010923</v>
+        <v>0.1300240414387865</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2705,13 +2705,13 @@
         <v>137</v>
       </c>
       <c r="B135">
-        <v>81.5733624624034</v>
+        <v>129.4975258173286</v>
       </c>
       <c r="C135">
-        <v>-0.1879615892583018</v>
+        <v>-0.8858862983106111</v>
       </c>
       <c r="D135">
-        <v>0.02448365544641497</v>
+        <v>0.1318444385279162</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2719,13 +2719,13 @@
         <v>138</v>
       </c>
       <c r="B136">
-        <v>81.70222325461648</v>
+        <v>163.8315736903427</v>
       </c>
       <c r="C136">
-        <v>-0.1898382027371333</v>
+        <v>-1.385896704228291</v>
       </c>
       <c r="D136">
-        <v>0.1648050227775083</v>
+        <v>0.03010100558100193</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2733,13 +2733,13 @@
         <v>139</v>
       </c>
       <c r="B137">
-        <v>82.39457954768551</v>
+        <v>166.1277012754091</v>
       </c>
       <c r="C137">
-        <v>-0.199921061374061</v>
+        <v>-1.419335455467123</v>
       </c>
       <c r="D137">
-        <v>0.1474924304686204</v>
+        <v>0.1618111244979356</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2747,13 +2747,13 @@
         <v>140</v>
       </c>
       <c r="B138">
-        <v>84.89786533478514</v>
+        <v>187.800331913914</v>
       </c>
       <c r="C138">
-        <v>-0.2363766796327933</v>
+        <v>-1.734956290008455</v>
       </c>
       <c r="D138">
-        <v>0.1103243880336632</v>
+        <v>0.1518812186638858</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -2761,13 +2761,13 @@
         <v>141</v>
       </c>
       <c r="B139">
-        <v>85.58381225072721</v>
+        <v>324.6058281413501</v>
       </c>
       <c r="C139">
-        <v>-0.2463661978261242</v>
+        <v>-3.727269341864321</v>
       </c>
       <c r="D139">
-        <v>0.5991233778310178</v>
+        <v>0.2578024523514668</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -2775,13 +2775,13 @@
         <v>142</v>
       </c>
       <c r="B140">
-        <v>85.66687333479064</v>
+        <v>617.6029945842153</v>
       </c>
       <c r="C140">
-        <v>-0.2475758252639413</v>
+        <v>-7.994218367731291</v>
       </c>
       <c r="D140">
-        <v>0.1160707500643826</v>
+        <v>0.03019927070465828</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2789,13 +2789,13 @@
         <v>143</v>
       </c>
       <c r="B141">
-        <v>85.78251485107938</v>
+        <v>21808.64432629243</v>
       </c>
       <c r="C141">
-        <v>-0.2492599250157193</v>
+        <v>-316.6016164023169</v>
       </c>
       <c r="D141">
-        <v>0.2566469433622143</v>
+        <v>0.02427179035916842</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -2803,13 +2803,13 @@
         <v>144</v>
       </c>
       <c r="B142">
-        <v>86.82709156694065</v>
+        <v>25424.30176986883</v>
       </c>
       <c r="C142">
-        <v>-0.2644722072855434</v>
+        <v>-369.2568218912936</v>
       </c>
       <c r="D142">
-        <v>0.02674639247359616</v>
+        <v>0.02691530840072508</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2817,13 +2817,13 @@
         <v>145</v>
       </c>
       <c r="B143">
-        <v>87.01850664548199</v>
+        <v>13807525.38829923</v>
       </c>
       <c r="C143">
-        <v>-0.2672598055167281</v>
+        <v>-201079.4668198917</v>
       </c>
       <c r="D143">
-        <v>0.01428537148615574</v>
+        <v>0.02556496413792915</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2831,13 +2831,13 @@
         <v>146</v>
       </c>
       <c r="B144">
-        <v>87.02785486205696</v>
+        <v>13807525.38829923</v>
       </c>
       <c r="C144">
-        <v>-0.2673959445930625</v>
+        <v>-201079.4668198917</v>
       </c>
       <c r="D144">
-        <v>0.008859584317472918</v>
+        <v>0.0255649641379294</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2845,13 +2845,13 @@
         <v>147</v>
       </c>
       <c r="B145">
-        <v>94.01262756916685</v>
+        <v>53705000.61247429</v>
       </c>
       <c r="C145">
-        <v>-0.3691159354733036</v>
+        <v>-782110.6594049652</v>
       </c>
       <c r="D145">
-        <v>0.1115121138368898</v>
+        <v>0.02551338187177616</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2859,13 +2859,13 @@
         <v>148</v>
       </c>
       <c r="B146">
-        <v>94.62876210502735</v>
+        <v>53877814.06218128</v>
       </c>
       <c r="C146">
-        <v>-0.3780887685198158</v>
+        <v>-784627.3601288536</v>
       </c>
       <c r="D146">
-        <v>0.02967969138440198</v>
+        <v>0.02556864373089735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>